<commit_message>
Best time to buy and sell stocks
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Placements\Love-Babbar-SDE-Sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82C4C2CF-D494-48B7-9029-74A8390A8F39}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E78B47F-62CE-4DDD-80A8-C1964CC2C538}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1429,7 +1429,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1509,8 +1509,13 @@
       <color theme="10"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1520,6 +1525,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1536,7 +1547,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1568,6 +1579,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1787,8 +1801,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A145" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.1796875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2061,7 +2075,7 @@
       <c r="C22" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="D22" s="5" t="s">
+      <c r="D22" s="18" t="s">
         <v>8</v>
       </c>
     </row>
@@ -2075,7 +2089,7 @@
       <c r="C23" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="D23" s="5" t="s">
+      <c r="D23" s="19" t="s">
         <v>8</v>
       </c>
     </row>
@@ -8658,6 +8672,6 @@
     <hyperlink ref="C481" r:id="rId446" xr:uid="{00000000-0004-0000-0000-0000BD010000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup orientation="portrait" r:id="rId447"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Sortlist Leetcode divide and Conquer
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Placements\Love-Babbar-SDE-Sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E78B47F-62CE-4DDD-80A8-C1964CC2C538}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8DB9661-269A-4FC4-A3E1-20A118E4305F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1350" uniqueCount="466">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1350" uniqueCount="465">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -439,9 +439,6 @@
   </si>
   <si>
     <t>Write a Program to reverse the Linked List. (Both Iterative and recursive)</t>
-  </si>
-  <si>
-    <t>Reverse a Linked List in group of Given Size. [Very Imp]</t>
   </si>
   <si>
     <t>Write a program to Detect loop in a linked list.</t>
@@ -1801,8 +1798,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D481"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" topLeftCell="A294" workbookViewId="0">
+      <selection activeCell="C479" sqref="C479"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.1796875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3628,7 +3625,7 @@
       <c r="C139" s="8" t="s">
         <v>137</v>
       </c>
-      <c r="D139" s="5" t="s">
+      <c r="D139" s="18" t="s">
         <v>8</v>
       </c>
     </row>
@@ -3640,7 +3637,7 @@
         <v>136</v>
       </c>
       <c r="C140" s="8" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D140" s="5" t="s">
         <v>8</v>
@@ -3654,7 +3651,7 @@
         <v>136</v>
       </c>
       <c r="C141" s="8" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D141" s="5" t="s">
         <v>8</v>
@@ -3668,7 +3665,7 @@
         <v>136</v>
       </c>
       <c r="C142" s="8" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D142" s="5" t="s">
         <v>8</v>
@@ -3682,7 +3679,7 @@
         <v>136</v>
       </c>
       <c r="C143" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D143" s="5" t="s">
         <v>8</v>
@@ -3696,7 +3693,7 @@
         <v>136</v>
       </c>
       <c r="C144" s="8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D144" s="5" t="s">
         <v>8</v>
@@ -3710,7 +3707,7 @@
         <v>136</v>
       </c>
       <c r="C145" s="8" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D145" s="5" t="s">
         <v>8</v>
@@ -3724,7 +3721,7 @@
         <v>136</v>
       </c>
       <c r="C146" s="8" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D146" s="5" t="s">
         <v>8</v>
@@ -3738,7 +3735,7 @@
         <v>136</v>
       </c>
       <c r="C147" s="8" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D147" s="5" t="s">
         <v>8</v>
@@ -3752,7 +3749,7 @@
         <v>136</v>
       </c>
       <c r="C148" s="8" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D148" s="5" t="s">
         <v>8</v>
@@ -3766,7 +3763,7 @@
         <v>136</v>
       </c>
       <c r="C149" s="8" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D149" s="5" t="s">
         <v>8</v>
@@ -3780,7 +3777,7 @@
         <v>136</v>
       </c>
       <c r="C150" s="8" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D150" s="5" t="s">
         <v>8</v>
@@ -3794,7 +3791,7 @@
         <v>136</v>
       </c>
       <c r="C151" s="8" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D151" s="5" t="s">
         <v>8</v>
@@ -3808,7 +3805,7 @@
         <v>136</v>
       </c>
       <c r="C152" s="8" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D152" s="5" t="s">
         <v>8</v>
@@ -3822,7 +3819,7 @@
         <v>136</v>
       </c>
       <c r="C153" s="8" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D153" s="5" t="s">
         <v>8</v>
@@ -3836,7 +3833,7 @@
         <v>136</v>
       </c>
       <c r="C154" s="8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D154" s="5" t="s">
         <v>8</v>
@@ -3850,7 +3847,7 @@
         <v>136</v>
       </c>
       <c r="C155" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D155" s="5" t="s">
         <v>8</v>
@@ -3864,7 +3861,7 @@
         <v>136</v>
       </c>
       <c r="C156" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D156" s="5" t="s">
         <v>8</v>
@@ -3878,7 +3875,7 @@
         <v>136</v>
       </c>
       <c r="C157" s="8" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D157" s="5" t="s">
         <v>8</v>
@@ -3892,7 +3889,7 @@
         <v>136</v>
       </c>
       <c r="C158" s="8" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D158" s="5" t="s">
         <v>8</v>
@@ -3906,7 +3903,7 @@
         <v>136</v>
       </c>
       <c r="C159" s="8" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D159" s="5" t="s">
         <v>8</v>
@@ -3920,7 +3917,7 @@
         <v>136</v>
       </c>
       <c r="C160" s="8" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D160" s="5" t="s">
         <v>8</v>
@@ -3934,7 +3931,7 @@
         <v>136</v>
       </c>
       <c r="C161" s="8" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D161" s="5" t="s">
         <v>8</v>
@@ -3948,7 +3945,7 @@
         <v>136</v>
       </c>
       <c r="C162" s="8" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D162" s="5" t="s">
         <v>8</v>
@@ -3962,7 +3959,7 @@
         <v>136</v>
       </c>
       <c r="C163" s="8" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D163" s="5" t="s">
         <v>8</v>
@@ -3976,7 +3973,7 @@
         <v>136</v>
       </c>
       <c r="C164" s="10" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D164" s="5" t="s">
         <v>8</v>
@@ -3990,7 +3987,7 @@
         <v>136</v>
       </c>
       <c r="C165" s="10" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D165" s="5" t="s">
         <v>8</v>
@@ -4004,7 +4001,7 @@
         <v>136</v>
       </c>
       <c r="C166" s="8" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D166" s="5" t="s">
         <v>8</v>
@@ -4018,7 +4015,7 @@
         <v>136</v>
       </c>
       <c r="C167" s="8" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D167" s="5" t="s">
         <v>8</v>
@@ -4032,7 +4029,7 @@
         <v>136</v>
       </c>
       <c r="C168" s="8" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D168" s="5" t="s">
         <v>8</v>
@@ -4046,7 +4043,7 @@
         <v>136</v>
       </c>
       <c r="C169" s="8" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D169" s="5" t="s">
         <v>8</v>
@@ -4060,7 +4057,7 @@
         <v>136</v>
       </c>
       <c r="C170" s="8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D170" s="5" t="s">
         <v>8</v>
@@ -4074,7 +4071,7 @@
         <v>136</v>
       </c>
       <c r="C171" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D171" s="5" t="s">
         <v>8</v>
@@ -4088,7 +4085,7 @@
         <v>136</v>
       </c>
       <c r="C172" s="8" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D172" s="5" t="s">
         <v>8</v>
@@ -4102,7 +4099,7 @@
         <v>136</v>
       </c>
       <c r="C173" s="8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D173" s="5" t="s">
         <v>8</v>
@@ -4116,7 +4113,7 @@
         <v>136</v>
       </c>
       <c r="C174" s="8" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D174" s="5" t="s">
         <v>8</v>
@@ -4132,10 +4129,10 @@
         <v>162</v>
       </c>
       <c r="B177" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="C177" s="8" t="s">
         <v>173</v>
-      </c>
-      <c r="C177" s="8" t="s">
-        <v>174</v>
       </c>
       <c r="D177" s="5" t="s">
         <v>8</v>
@@ -4146,10 +4143,10 @@
         <v>163</v>
       </c>
       <c r="B178" s="7" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C178" s="8" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D178" s="5" t="s">
         <v>8</v>
@@ -4160,10 +4157,10 @@
         <v>164</v>
       </c>
       <c r="B179" s="7" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C179" s="8" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D179" s="5" t="s">
         <v>8</v>
@@ -4174,10 +4171,10 @@
         <v>165</v>
       </c>
       <c r="B180" s="7" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C180" s="8" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D180" s="5" t="s">
         <v>8</v>
@@ -4188,10 +4185,10 @@
         <v>166</v>
       </c>
       <c r="B181" s="7" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C181" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D181" s="5" t="s">
         <v>8</v>
@@ -4202,10 +4199,10 @@
         <v>167</v>
       </c>
       <c r="B182" s="7" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C182" s="8" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D182" s="5" t="s">
         <v>8</v>
@@ -4216,10 +4213,10 @@
         <v>168</v>
       </c>
       <c r="B183" s="7" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C183" s="8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D183" s="5" t="s">
         <v>8</v>
@@ -4230,10 +4227,10 @@
         <v>169</v>
       </c>
       <c r="B184" s="7" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C184" s="8" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D184" s="5" t="s">
         <v>8</v>
@@ -4244,10 +4241,10 @@
         <v>170</v>
       </c>
       <c r="B185" s="7" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C185" s="8" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D185" s="5" t="s">
         <v>8</v>
@@ -4258,10 +4255,10 @@
         <v>171</v>
       </c>
       <c r="B186" s="7" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C186" s="8" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D186" s="5" t="s">
         <v>8</v>
@@ -4272,10 +4269,10 @@
         <v>172</v>
       </c>
       <c r="B187" s="7" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C187" s="8" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D187" s="5" t="s">
         <v>8</v>
@@ -4286,10 +4283,10 @@
         <v>173</v>
       </c>
       <c r="B188" s="7" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C188" s="8" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D188" s="5" t="s">
         <v>8</v>
@@ -4300,10 +4297,10 @@
         <v>174</v>
       </c>
       <c r="B189" s="7" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C189" s="8" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D189" s="5" t="s">
         <v>8</v>
@@ -4314,10 +4311,10 @@
         <v>175</v>
       </c>
       <c r="B190" s="7" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C190" s="8" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D190" s="5" t="s">
         <v>8</v>
@@ -4328,10 +4325,10 @@
         <v>176</v>
       </c>
       <c r="B191" s="7" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C191" s="8" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D191" s="5" t="s">
         <v>8</v>
@@ -4342,10 +4339,10 @@
         <v>177</v>
       </c>
       <c r="B192" s="7" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C192" s="8" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D192" s="5" t="s">
         <v>8</v>
@@ -4356,10 +4353,10 @@
         <v>178</v>
       </c>
       <c r="B193" s="7" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C193" s="8" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D193" s="5" t="s">
         <v>8</v>
@@ -4370,10 +4367,10 @@
         <v>179</v>
       </c>
       <c r="B194" s="7" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C194" s="8" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D194" s="5" t="s">
         <v>8</v>
@@ -4384,10 +4381,10 @@
         <v>180</v>
       </c>
       <c r="B195" s="7" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C195" s="8" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D195" s="5" t="s">
         <v>8</v>
@@ -4398,10 +4395,10 @@
         <v>181</v>
       </c>
       <c r="B196" s="7" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C196" s="8" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D196" s="5" t="s">
         <v>8</v>
@@ -4412,10 +4409,10 @@
         <v>182</v>
       </c>
       <c r="B197" s="7" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C197" s="8" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D197" s="5" t="s">
         <v>8</v>
@@ -4426,10 +4423,10 @@
         <v>183</v>
       </c>
       <c r="B198" s="7" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C198" s="8" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D198" s="5" t="s">
         <v>8</v>
@@ -4440,10 +4437,10 @@
         <v>184</v>
       </c>
       <c r="B199" s="7" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C199" s="8" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D199" s="5" t="s">
         <v>8</v>
@@ -4454,10 +4451,10 @@
         <v>185</v>
       </c>
       <c r="B200" s="7" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C200" s="8" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D200" s="5" t="s">
         <v>8</v>
@@ -4468,10 +4465,10 @@
         <v>186</v>
       </c>
       <c r="B201" s="7" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C201" s="8" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D201" s="5" t="s">
         <v>8</v>
@@ -4482,10 +4479,10 @@
         <v>187</v>
       </c>
       <c r="B202" s="7" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C202" s="8" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D202" s="5" t="s">
         <v>8</v>
@@ -4496,10 +4493,10 @@
         <v>188</v>
       </c>
       <c r="B203" s="7" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C203" s="8" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D203" s="5" t="s">
         <v>8</v>
@@ -4510,10 +4507,10 @@
         <v>189</v>
       </c>
       <c r="B204" s="7" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C204" s="8" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D204" s="5" t="s">
         <v>8</v>
@@ -4524,10 +4521,10 @@
         <v>190</v>
       </c>
       <c r="B205" s="7" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C205" s="8" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D205" s="5" t="s">
         <v>8</v>
@@ -4538,10 +4535,10 @@
         <v>191</v>
       </c>
       <c r="B206" s="7" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C206" s="8" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D206" s="5" t="s">
         <v>8</v>
@@ -4552,10 +4549,10 @@
         <v>192</v>
       </c>
       <c r="B207" s="7" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C207" s="8" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D207" s="5" t="s">
         <v>8</v>
@@ -4566,10 +4563,10 @@
         <v>193</v>
       </c>
       <c r="B208" s="7" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C208" s="8" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D208" s="5" t="s">
         <v>8</v>
@@ -4580,10 +4577,10 @@
         <v>194</v>
       </c>
       <c r="B209" s="7" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C209" s="8" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D209" s="5" t="s">
         <v>8</v>
@@ -4594,10 +4591,10 @@
         <v>195</v>
       </c>
       <c r="B210" s="7" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C210" s="8" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D210" s="5" t="s">
         <v>8</v>
@@ -4608,10 +4605,10 @@
         <v>196</v>
       </c>
       <c r="B211" s="7" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C211" s="8" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D211" s="5" t="s">
         <v>8</v>
@@ -4633,10 +4630,10 @@
         <v>197</v>
       </c>
       <c r="B214" s="7" t="s">
+        <v>208</v>
+      </c>
+      <c r="C214" s="8" t="s">
         <v>209</v>
-      </c>
-      <c r="C214" s="8" t="s">
-        <v>210</v>
       </c>
       <c r="D214" s="5" t="s">
         <v>8</v>
@@ -4647,10 +4644,10 @@
         <v>198</v>
       </c>
       <c r="B215" s="7" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C215" s="8" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D215" s="5" t="s">
         <v>8</v>
@@ -4661,10 +4658,10 @@
         <v>199</v>
       </c>
       <c r="B216" s="7" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C216" s="8" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D216" s="5" t="s">
         <v>8</v>
@@ -4675,10 +4672,10 @@
         <v>200</v>
       </c>
       <c r="B217" s="7" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C217" s="8" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D217" s="5" t="s">
         <v>8</v>
@@ -4689,10 +4686,10 @@
         <v>201</v>
       </c>
       <c r="B218" s="7" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C218" s="8" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D218" s="5" t="s">
         <v>8</v>
@@ -4703,10 +4700,10 @@
         <v>202</v>
       </c>
       <c r="B219" s="7" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C219" s="8" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D219" s="5" t="s">
         <v>8</v>
@@ -4717,10 +4714,10 @@
         <v>203</v>
       </c>
       <c r="B220" s="7" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C220" s="17" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D220" s="5" t="s">
         <v>8</v>
@@ -4731,10 +4728,10 @@
         <v>204</v>
       </c>
       <c r="B221" s="7" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C221" s="8" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D221" s="5" t="s">
         <v>8</v>
@@ -4745,10 +4742,10 @@
         <v>205</v>
       </c>
       <c r="B222" s="7" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C222" s="8" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D222" s="5" t="s">
         <v>8</v>
@@ -4759,10 +4756,10 @@
         <v>206</v>
       </c>
       <c r="B223" s="7" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C223" s="8" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D223" s="5" t="s">
         <v>8</v>
@@ -4773,10 +4770,10 @@
         <v>207</v>
       </c>
       <c r="B224" s="7" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C224" s="8" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D224" s="5" t="s">
         <v>8</v>
@@ -4787,10 +4784,10 @@
         <v>208</v>
       </c>
       <c r="B225" s="7" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C225" s="8" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D225" s="5" t="s">
         <v>8</v>
@@ -4801,10 +4798,10 @@
         <v>209</v>
       </c>
       <c r="B226" s="7" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C226" s="8" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D226" s="5" t="s">
         <v>8</v>
@@ -4815,10 +4812,10 @@
         <v>210</v>
       </c>
       <c r="B227" s="7" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C227" s="8" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D227" s="5" t="s">
         <v>8</v>
@@ -4829,10 +4826,10 @@
         <v>211</v>
       </c>
       <c r="B228" s="7" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C228" s="8" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D228" s="5" t="s">
         <v>8</v>
@@ -4843,10 +4840,10 @@
         <v>212</v>
       </c>
       <c r="B229" s="7" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C229" s="8" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D229" s="5" t="s">
         <v>8</v>
@@ -4857,10 +4854,10 @@
         <v>213</v>
       </c>
       <c r="B230" s="7" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C230" s="8" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D230" s="5" t="s">
         <v>8</v>
@@ -4871,10 +4868,10 @@
         <v>214</v>
       </c>
       <c r="B231" s="7" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C231" s="8" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D231" s="5" t="s">
         <v>8</v>
@@ -4885,10 +4882,10 @@
         <v>215</v>
       </c>
       <c r="B232" s="7" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C232" s="8" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D232" s="5" t="s">
         <v>8</v>
@@ -4899,10 +4896,10 @@
         <v>216</v>
       </c>
       <c r="B233" s="7" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C233" s="8" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D233" s="5" t="s">
         <v>8</v>
@@ -4913,10 +4910,10 @@
         <v>217</v>
       </c>
       <c r="B234" s="7" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C234" s="8" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D234" s="5" t="s">
         <v>8</v>
@@ -4927,10 +4924,10 @@
         <v>218</v>
       </c>
       <c r="B235" s="7" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C235" s="8" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D235" s="5" t="s">
         <v>8</v>
@@ -4949,10 +4946,10 @@
         <v>219</v>
       </c>
       <c r="B238" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="C238" s="8" t="s">
         <v>232</v>
-      </c>
-      <c r="C238" s="8" t="s">
-        <v>233</v>
       </c>
       <c r="D238" s="5" t="s">
         <v>8</v>
@@ -4963,10 +4960,10 @@
         <v>220</v>
       </c>
       <c r="B239" s="7" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C239" s="8" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D239" s="5" t="s">
         <v>8</v>
@@ -4977,10 +4974,10 @@
         <v>221</v>
       </c>
       <c r="B240" s="7" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C240" s="8" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D240" s="5" t="s">
         <v>8</v>
@@ -4991,10 +4988,10 @@
         <v>222</v>
       </c>
       <c r="B241" s="7" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C241" s="8" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D241" s="5" t="s">
         <v>8</v>
@@ -5005,10 +5002,10 @@
         <v>223</v>
       </c>
       <c r="B242" s="7" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C242" s="8" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D242" s="5" t="s">
         <v>8</v>
@@ -5019,10 +5016,10 @@
         <v>224</v>
       </c>
       <c r="B243" s="7" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C243" s="8" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D243" s="5" t="s">
         <v>8</v>
@@ -5033,10 +5030,10 @@
         <v>225</v>
       </c>
       <c r="B244" s="7" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C244" s="8" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D244" s="5" t="s">
         <v>8</v>
@@ -5047,10 +5044,10 @@
         <v>226</v>
       </c>
       <c r="B245" s="7" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C245" s="8" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D245" s="5" t="s">
         <v>8</v>
@@ -5061,10 +5058,10 @@
         <v>227</v>
       </c>
       <c r="B246" s="7" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C246" s="8" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D246" s="5" t="s">
         <v>8</v>
@@ -5075,10 +5072,10 @@
         <v>228</v>
       </c>
       <c r="B247" s="7" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C247" s="8" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D247" s="5" t="s">
         <v>8</v>
@@ -5089,10 +5086,10 @@
         <v>229</v>
       </c>
       <c r="B248" s="7" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C248" s="8" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D248" s="5" t="s">
         <v>8</v>
@@ -5103,10 +5100,10 @@
         <v>230</v>
       </c>
       <c r="B249" s="7" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C249" s="8" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D249" s="5" t="s">
         <v>8</v>
@@ -5117,10 +5114,10 @@
         <v>231</v>
       </c>
       <c r="B250" s="7" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C250" s="8" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D250" s="5" t="s">
         <v>8</v>
@@ -5131,10 +5128,10 @@
         <v>232</v>
       </c>
       <c r="B251" s="7" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C251" s="8" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D251" s="5" t="s">
         <v>8</v>
@@ -5145,10 +5142,10 @@
         <v>233</v>
       </c>
       <c r="B252" s="7" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C252" s="8" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D252" s="5" t="s">
         <v>8</v>
@@ -5159,10 +5156,10 @@
         <v>234</v>
       </c>
       <c r="B253" s="7" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C253" s="8" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D253" s="5" t="s">
         <v>8</v>
@@ -5173,10 +5170,10 @@
         <v>235</v>
       </c>
       <c r="B254" s="7" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C254" s="8" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D254" s="5" t="s">
         <v>8</v>
@@ -5187,10 +5184,10 @@
         <v>236</v>
       </c>
       <c r="B255" s="7" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C255" s="8" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D255" s="5" t="s">
         <v>8</v>
@@ -5201,10 +5198,10 @@
         <v>237</v>
       </c>
       <c r="B256" s="7" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C256" s="8" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D256" s="5" t="s">
         <v>8</v>
@@ -5215,10 +5212,10 @@
         <v>238</v>
       </c>
       <c r="B257" s="7" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C257" s="8" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D257" s="5" t="s">
         <v>8</v>
@@ -5229,10 +5226,10 @@
         <v>239</v>
       </c>
       <c r="B258" s="7" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C258" s="8" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D258" s="5" t="s">
         <v>8</v>
@@ -5243,10 +5240,10 @@
         <v>240</v>
       </c>
       <c r="B259" s="7" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C259" s="8" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D259" s="5" t="s">
         <v>8</v>
@@ -5257,10 +5254,10 @@
         <v>241</v>
       </c>
       <c r="B260" s="7" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C260" s="8" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D260" s="5" t="s">
         <v>8</v>
@@ -5271,10 +5268,10 @@
         <v>242</v>
       </c>
       <c r="B261" s="7" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C261" s="8" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D261" s="5" t="s">
         <v>8</v>
@@ -5285,10 +5282,10 @@
         <v>243</v>
       </c>
       <c r="B262" s="7" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C262" s="8" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D262" s="5" t="s">
         <v>8</v>
@@ -5299,10 +5296,10 @@
         <v>244</v>
       </c>
       <c r="B263" s="7" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C263" s="8" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D263" s="5" t="s">
         <v>8</v>
@@ -5313,10 +5310,10 @@
         <v>245</v>
       </c>
       <c r="B264" s="7" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C264" s="8" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D264" s="5" t="s">
         <v>8</v>
@@ -5327,10 +5324,10 @@
         <v>246</v>
       </c>
       <c r="B265" s="7" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C265" s="8" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D265" s="5" t="s">
         <v>8</v>
@@ -5341,10 +5338,10 @@
         <v>247</v>
       </c>
       <c r="B266" s="7" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C266" s="8" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D266" s="5" t="s">
         <v>8</v>
@@ -5355,10 +5352,10 @@
         <v>248</v>
       </c>
       <c r="B267" s="7" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C267" s="8" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D267" s="5" t="s">
         <v>8</v>
@@ -5369,10 +5366,10 @@
         <v>249</v>
       </c>
       <c r="B268" s="7" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C268" s="8" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D268" s="5" t="s">
         <v>8</v>
@@ -5383,10 +5380,10 @@
         <v>250</v>
       </c>
       <c r="B269" s="7" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C269" s="8" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D269" s="5" t="s">
         <v>8</v>
@@ -5397,10 +5394,10 @@
         <v>251</v>
       </c>
       <c r="B270" s="7" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C270" s="8" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D270" s="5" t="s">
         <v>8</v>
@@ -5411,7 +5408,7 @@
         <v>252</v>
       </c>
       <c r="B271" s="7" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C271" s="8" t="s">
         <v>89</v>
@@ -5425,10 +5422,10 @@
         <v>253</v>
       </c>
       <c r="B272" s="7" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C272" s="8" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D272" s="5" t="s">
         <v>8</v>
@@ -5447,10 +5444,10 @@
         <v>254</v>
       </c>
       <c r="B275" s="7" t="s">
+        <v>266</v>
+      </c>
+      <c r="C275" s="8" t="s">
         <v>267</v>
-      </c>
-      <c r="C275" s="8" t="s">
-        <v>268</v>
       </c>
       <c r="D275" s="5" t="s">
         <v>8</v>
@@ -5461,10 +5458,10 @@
         <v>255</v>
       </c>
       <c r="B276" s="7" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C276" s="8" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D276" s="5" t="s">
         <v>8</v>
@@ -5475,10 +5472,10 @@
         <v>256</v>
       </c>
       <c r="B277" s="7" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C277" s="8" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D277" s="5" t="s">
         <v>8</v>
@@ -5489,10 +5486,10 @@
         <v>257</v>
       </c>
       <c r="B278" s="7" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C278" s="8" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D278" s="5" t="s">
         <v>8</v>
@@ -5503,10 +5500,10 @@
         <v>258</v>
       </c>
       <c r="B279" s="7" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C279" s="8" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D279" s="5" t="s">
         <v>8</v>
@@ -5517,10 +5514,10 @@
         <v>259</v>
       </c>
       <c r="B280" s="7" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C280" s="8" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D280" s="5" t="s">
         <v>8</v>
@@ -5531,10 +5528,10 @@
         <v>260</v>
       </c>
       <c r="B281" s="7" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C281" s="8" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D281" s="5" t="s">
         <v>8</v>
@@ -5545,10 +5542,10 @@
         <v>261</v>
       </c>
       <c r="B282" s="7" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C282" s="8" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D282" s="5" t="s">
         <v>8</v>
@@ -5559,10 +5556,10 @@
         <v>262</v>
       </c>
       <c r="B283" s="7" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C283" s="8" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D283" s="5" t="s">
         <v>8</v>
@@ -5573,10 +5570,10 @@
         <v>263</v>
       </c>
       <c r="B284" s="7" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C284" s="8" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D284" s="5" t="s">
         <v>8</v>
@@ -5587,10 +5584,10 @@
         <v>264</v>
       </c>
       <c r="B285" s="7" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C285" s="8" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D285" s="5" t="s">
         <v>8</v>
@@ -5601,10 +5598,10 @@
         <v>265</v>
       </c>
       <c r="B286" s="7" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C286" s="8" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D286" s="5" t="s">
         <v>8</v>
@@ -5615,10 +5612,10 @@
         <v>266</v>
       </c>
       <c r="B287" s="7" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C287" s="8" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D287" s="5" t="s">
         <v>8</v>
@@ -5629,10 +5626,10 @@
         <v>267</v>
       </c>
       <c r="B288" s="7" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C288" s="8" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D288" s="5" t="s">
         <v>8</v>
@@ -5643,10 +5640,10 @@
         <v>268</v>
       </c>
       <c r="B289" s="7" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C289" s="8" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D289" s="5" t="s">
         <v>8</v>
@@ -5657,10 +5654,10 @@
         <v>269</v>
       </c>
       <c r="B290" s="7" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C290" s="8" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D290" s="5" t="s">
         <v>8</v>
@@ -5671,10 +5668,10 @@
         <v>270</v>
       </c>
       <c r="B291" s="7" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C291" s="8" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D291" s="5" t="s">
         <v>8</v>
@@ -5685,10 +5682,10 @@
         <v>271</v>
       </c>
       <c r="B292" s="7" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C292" s="8" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D292" s="5" t="s">
         <v>8</v>
@@ -5699,10 +5696,10 @@
         <v>272</v>
       </c>
       <c r="B293" s="7" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C293" s="8" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D293" s="5" t="s">
         <v>8</v>
@@ -5721,10 +5718,10 @@
         <v>273</v>
       </c>
       <c r="B296" s="7" t="s">
+        <v>286</v>
+      </c>
+      <c r="C296" s="8" t="s">
         <v>287</v>
-      </c>
-      <c r="C296" s="8" t="s">
-        <v>288</v>
       </c>
       <c r="D296" s="5" t="s">
         <v>8</v>
@@ -5735,10 +5732,10 @@
         <v>274</v>
       </c>
       <c r="B297" s="7" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C297" s="8" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D297" s="5" t="s">
         <v>8</v>
@@ -5749,10 +5746,10 @@
         <v>275</v>
       </c>
       <c r="B298" s="7" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C298" s="8" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D298" s="5" t="s">
         <v>8</v>
@@ -5763,10 +5760,10 @@
         <v>276</v>
       </c>
       <c r="B299" s="7" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C299" s="8" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="D299" s="5" t="s">
         <v>8</v>
@@ -5777,10 +5774,10 @@
         <v>277</v>
       </c>
       <c r="B300" s="7" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C300" s="8" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D300" s="5" t="s">
         <v>8</v>
@@ -5791,10 +5788,10 @@
         <v>278</v>
       </c>
       <c r="B301" s="7" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C301" s="8" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="D301" s="5" t="s">
         <v>8</v>
@@ -5805,10 +5802,10 @@
         <v>279</v>
       </c>
       <c r="B302" s="7" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C302" s="8" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D302" s="5" t="s">
         <v>8</v>
@@ -5819,10 +5816,10 @@
         <v>280</v>
       </c>
       <c r="B303" s="7" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C303" s="8" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D303" s="5" t="s">
         <v>8</v>
@@ -5833,10 +5830,10 @@
         <v>281</v>
       </c>
       <c r="B304" s="7" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C304" s="8" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D304" s="5" t="s">
         <v>8</v>
@@ -5847,10 +5844,10 @@
         <v>282</v>
       </c>
       <c r="B305" s="7" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C305" s="8" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D305" s="5" t="s">
         <v>8</v>
@@ -5861,10 +5858,10 @@
         <v>283</v>
       </c>
       <c r="B306" s="7" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C306" s="8" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D306" s="5" t="s">
         <v>8</v>
@@ -5875,10 +5872,10 @@
         <v>284</v>
       </c>
       <c r="B307" s="7" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C307" s="8" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D307" s="5" t="s">
         <v>8</v>
@@ -5889,10 +5886,10 @@
         <v>285</v>
       </c>
       <c r="B308" s="7" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C308" s="8" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="D308" s="5" t="s">
         <v>8</v>
@@ -5903,10 +5900,10 @@
         <v>286</v>
       </c>
       <c r="B309" s="7" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C309" s="17" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D309" s="5" t="s">
         <v>8</v>
@@ -5917,10 +5914,10 @@
         <v>287</v>
       </c>
       <c r="B310" s="7" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C310" s="8" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D310" s="5" t="s">
         <v>8</v>
@@ -5931,10 +5928,10 @@
         <v>288</v>
       </c>
       <c r="B311" s="7" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C311" s="8" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D311" s="5" t="s">
         <v>8</v>
@@ -5945,10 +5942,10 @@
         <v>289</v>
       </c>
       <c r="B312" s="7" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C312" s="8" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D312" s="5" t="s">
         <v>8</v>
@@ -5959,10 +5956,10 @@
         <v>290</v>
       </c>
       <c r="B313" s="7" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C313" s="8" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D313" s="5" t="s">
         <v>8</v>
@@ -5973,10 +5970,10 @@
         <v>291</v>
       </c>
       <c r="B314" s="7" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C314" s="8" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D314" s="5" t="s">
         <v>8</v>
@@ -5987,10 +5984,10 @@
         <v>292</v>
       </c>
       <c r="B315" s="7" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C315" s="8" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D315" s="5" t="s">
         <v>8</v>
@@ -6001,10 +5998,10 @@
         <v>293</v>
       </c>
       <c r="B316" s="7" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C316" s="8" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D316" s="5" t="s">
         <v>8</v>
@@ -6015,10 +6012,10 @@
         <v>294</v>
       </c>
       <c r="B317" s="7" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C317" s="8" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D317" s="5" t="s">
         <v>8</v>
@@ -6029,10 +6026,10 @@
         <v>295</v>
       </c>
       <c r="B318" s="7" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C318" s="8" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D318" s="5" t="s">
         <v>8</v>
@@ -6043,10 +6040,10 @@
         <v>296</v>
       </c>
       <c r="B319" s="7" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C319" s="8" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D319" s="5" t="s">
         <v>8</v>
@@ -6057,10 +6054,10 @@
         <v>297</v>
       </c>
       <c r="B320" s="7" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C320" s="8" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D320" s="5" t="s">
         <v>8</v>
@@ -6071,10 +6068,10 @@
         <v>298</v>
       </c>
       <c r="B321" s="7" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C321" s="8" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D321" s="5" t="s">
         <v>8</v>
@@ -6085,10 +6082,10 @@
         <v>299</v>
       </c>
       <c r="B322" s="7" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C322" s="8" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D322" s="5" t="s">
         <v>8</v>
@@ -6099,10 +6096,10 @@
         <v>300</v>
       </c>
       <c r="B323" s="7" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C323" s="8" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D323" s="5" t="s">
         <v>8</v>
@@ -6113,10 +6110,10 @@
         <v>301</v>
       </c>
       <c r="B324" s="7" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C324" s="8" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="D324" s="5" t="s">
         <v>8</v>
@@ -6127,10 +6124,10 @@
         <v>302</v>
       </c>
       <c r="B325" s="7" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C325" s="8" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="D325" s="5" t="s">
         <v>8</v>
@@ -6141,10 +6138,10 @@
         <v>303</v>
       </c>
       <c r="B326" s="7" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C326" s="8" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="D326" s="5" t="s">
         <v>8</v>
@@ -6155,10 +6152,10 @@
         <v>304</v>
       </c>
       <c r="B327" s="7" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C327" s="8" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="D327" s="5" t="s">
         <v>8</v>
@@ -6169,10 +6166,10 @@
         <v>305</v>
       </c>
       <c r="B328" s="7" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C328" s="8" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="D328" s="5" t="s">
         <v>8</v>
@@ -6183,10 +6180,10 @@
         <v>306</v>
       </c>
       <c r="B329" s="7" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C329" s="8" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="D329" s="5" t="s">
         <v>8</v>
@@ -6197,10 +6194,10 @@
         <v>307</v>
       </c>
       <c r="B330" s="7" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C330" s="8" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D330" s="5" t="s">
         <v>8</v>
@@ -6211,10 +6208,10 @@
         <v>308</v>
       </c>
       <c r="B331" s="7" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C331" s="8" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="D331" s="5" t="s">
         <v>8</v>
@@ -6225,10 +6222,10 @@
         <v>309</v>
       </c>
       <c r="B332" s="7" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C332" s="8" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="D332" s="5" t="s">
         <v>8</v>
@@ -6239,10 +6236,10 @@
         <v>310</v>
       </c>
       <c r="B333" s="7" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C333" s="8" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="D333" s="5" t="s">
         <v>8</v>
@@ -6261,10 +6258,10 @@
         <v>311</v>
       </c>
       <c r="B336" s="12" t="s">
+        <v>325</v>
+      </c>
+      <c r="C336" s="8" t="s">
         <v>326</v>
-      </c>
-      <c r="C336" s="8" t="s">
-        <v>327</v>
       </c>
       <c r="D336" s="5" t="s">
         <v>8</v>
@@ -6275,10 +6272,10 @@
         <v>312</v>
       </c>
       <c r="B337" s="12" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C337" s="8" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="D337" s="5" t="s">
         <v>8</v>
@@ -6289,10 +6286,10 @@
         <v>313</v>
       </c>
       <c r="B338" s="12" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C338" s="8" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="D338" s="5" t="s">
         <v>8</v>
@@ -6303,10 +6300,10 @@
         <v>314</v>
       </c>
       <c r="B339" s="12" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C339" s="8" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D339" s="5" t="s">
         <v>8</v>
@@ -6317,10 +6314,10 @@
         <v>315</v>
       </c>
       <c r="B340" s="12" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C340" s="8" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D340" s="5" t="s">
         <v>8</v>
@@ -6331,10 +6328,10 @@
         <v>316</v>
       </c>
       <c r="B341" s="12" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C341" s="8" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D341" s="5" t="s">
         <v>8</v>
@@ -6345,10 +6342,10 @@
         <v>317</v>
       </c>
       <c r="B342" s="12" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C342" s="8" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="D342" s="5" t="s">
         <v>8</v>
@@ -6359,10 +6356,10 @@
         <v>318</v>
       </c>
       <c r="B343" s="12" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C343" s="8" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="D343" s="5" t="s">
         <v>8</v>
@@ -6373,10 +6370,10 @@
         <v>319</v>
       </c>
       <c r="B344" s="12" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C344" s="17" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="D344" s="5" t="s">
         <v>8</v>
@@ -6387,10 +6384,10 @@
         <v>320</v>
       </c>
       <c r="B345" s="12" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C345" s="8" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="D345" s="5" t="s">
         <v>8</v>
@@ -6401,10 +6398,10 @@
         <v>321</v>
       </c>
       <c r="B346" s="12" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C346" s="8" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="D346" s="5" t="s">
         <v>8</v>
@@ -6415,10 +6412,10 @@
         <v>322</v>
       </c>
       <c r="B347" s="12" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C347" s="8" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="D347" s="5" t="s">
         <v>8</v>
@@ -6429,10 +6426,10 @@
         <v>323</v>
       </c>
       <c r="B348" s="12" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C348" s="8" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="D348" s="5" t="s">
         <v>8</v>
@@ -6443,10 +6440,10 @@
         <v>324</v>
       </c>
       <c r="B349" s="12" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C349" s="8" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="D349" s="5" t="s">
         <v>8</v>
@@ -6457,10 +6454,10 @@
         <v>325</v>
       </c>
       <c r="B350" s="12" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C350" s="8" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="D350" s="5" t="s">
         <v>8</v>
@@ -6471,10 +6468,10 @@
         <v>326</v>
       </c>
       <c r="B351" s="12" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C351" s="8" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="D351" s="5" t="s">
         <v>8</v>
@@ -6485,10 +6482,10 @@
         <v>327</v>
       </c>
       <c r="B352" s="12" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C352" s="8" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D352" s="5" t="s">
         <v>8</v>
@@ -6499,10 +6496,10 @@
         <v>328</v>
       </c>
       <c r="B353" s="12" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C353" s="8" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D353" s="5" t="s">
         <v>8</v>
@@ -6521,10 +6518,10 @@
         <v>329</v>
       </c>
       <c r="B356" s="12" t="s">
+        <v>344</v>
+      </c>
+      <c r="C356" s="8" t="s">
         <v>345</v>
-      </c>
-      <c r="C356" s="8" t="s">
-        <v>346</v>
       </c>
       <c r="D356" s="5" t="s">
         <v>8</v>
@@ -6535,10 +6532,10 @@
         <v>330</v>
       </c>
       <c r="B357" s="12" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C357" s="8" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D357" s="5" t="s">
         <v>8</v>
@@ -6549,10 +6546,10 @@
         <v>331</v>
       </c>
       <c r="B358" s="12" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C358" s="8" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D358" s="5" t="s">
         <v>8</v>
@@ -6563,10 +6560,10 @@
         <v>332</v>
       </c>
       <c r="B359" s="12" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C359" s="8" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D359" s="5" t="s">
         <v>8</v>
@@ -6577,10 +6574,10 @@
         <v>333</v>
       </c>
       <c r="B360" s="12" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C360" s="8" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="D360" s="5" t="s">
         <v>8</v>
@@ -6591,10 +6588,10 @@
         <v>334</v>
       </c>
       <c r="B361" s="12" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C361" s="8" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="D361" s="5" t="s">
         <v>8</v>
@@ -6605,10 +6602,10 @@
         <v>335</v>
       </c>
       <c r="B362" s="12" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C362" s="8" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="D362" s="5" t="s">
         <v>8</v>
@@ -6619,10 +6616,10 @@
         <v>336</v>
       </c>
       <c r="B363" s="12" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C363" s="8" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="D363" s="5" t="s">
         <v>8</v>
@@ -6633,10 +6630,10 @@
         <v>337</v>
       </c>
       <c r="B364" s="12" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C364" s="8" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="D364" s="5" t="s">
         <v>8</v>
@@ -6647,10 +6644,10 @@
         <v>338</v>
       </c>
       <c r="B365" s="12" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C365" s="8" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="D365" s="5" t="s">
         <v>8</v>
@@ -6661,10 +6658,10 @@
         <v>339</v>
       </c>
       <c r="B366" s="12" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C366" s="8" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="D366" s="5" t="s">
         <v>8</v>
@@ -6675,10 +6672,10 @@
         <v>340</v>
       </c>
       <c r="B367" s="12" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C367" s="8" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="D367" s="5" t="s">
         <v>8</v>
@@ -6689,10 +6686,10 @@
         <v>341</v>
       </c>
       <c r="B368" s="12" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C368" s="8" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="D368" s="5" t="s">
         <v>8</v>
@@ -6703,10 +6700,10 @@
         <v>342</v>
       </c>
       <c r="B369" s="12" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C369" s="8" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="D369" s="5" t="s">
         <v>8</v>
@@ -6717,10 +6714,10 @@
         <v>343</v>
       </c>
       <c r="B370" s="12" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C370" s="8" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="D370" s="5" t="s">
         <v>8</v>
@@ -6731,10 +6728,10 @@
         <v>344</v>
       </c>
       <c r="B371" s="12" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C371" s="8" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="D371" s="5" t="s">
         <v>8</v>
@@ -6745,10 +6742,10 @@
         <v>345</v>
       </c>
       <c r="B372" s="12" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C372" s="8" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="D372" s="5" t="s">
         <v>8</v>
@@ -6759,10 +6756,10 @@
         <v>346</v>
       </c>
       <c r="B373" s="12" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C373" s="8" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="D373" s="5" t="s">
         <v>8</v>
@@ -6773,10 +6770,10 @@
         <v>347</v>
       </c>
       <c r="B374" s="12" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C374" s="8" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="D374" s="5" t="s">
         <v>8</v>
@@ -6787,10 +6784,10 @@
         <v>348</v>
       </c>
       <c r="B375" s="12" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C375" s="8" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="D375" s="5" t="s">
         <v>8</v>
@@ -6801,10 +6798,10 @@
         <v>349</v>
       </c>
       <c r="B376" s="12" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C376" s="8" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="D376" s="5" t="s">
         <v>8</v>
@@ -6815,10 +6812,10 @@
         <v>350</v>
       </c>
       <c r="B377" s="12" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C377" s="8" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="D377" s="5" t="s">
         <v>8</v>
@@ -6829,10 +6826,10 @@
         <v>351</v>
       </c>
       <c r="B378" s="12" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C378" s="8" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="D378" s="5" t="s">
         <v>8</v>
@@ -6843,10 +6840,10 @@
         <v>352</v>
       </c>
       <c r="B379" s="12" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C379" s="8" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="D379" s="5" t="s">
         <v>8</v>
@@ -6857,10 +6854,10 @@
         <v>353</v>
       </c>
       <c r="B380" s="12" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C380" s="8" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="D380" s="5" t="s">
         <v>8</v>
@@ -6871,10 +6868,10 @@
         <v>354</v>
       </c>
       <c r="B381" s="12" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C381" s="8" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="D381" s="5" t="s">
         <v>8</v>
@@ -6885,10 +6882,10 @@
         <v>355</v>
       </c>
       <c r="B382" s="12" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C382" s="8" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="D382" s="5" t="s">
         <v>8</v>
@@ -6899,10 +6896,10 @@
         <v>356</v>
       </c>
       <c r="B383" s="12" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C383" s="8" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="D383" s="5" t="s">
         <v>8</v>
@@ -6913,10 +6910,10 @@
         <v>357</v>
       </c>
       <c r="B384" s="12" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C384" s="8" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="D384" s="5" t="s">
         <v>8</v>
@@ -6927,10 +6924,10 @@
         <v>358</v>
       </c>
       <c r="B385" s="12" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C385" s="8" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="D385" s="5" t="s">
         <v>8</v>
@@ -6941,10 +6938,10 @@
         <v>359</v>
       </c>
       <c r="B386" s="12" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C386" s="8" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="D386" s="5" t="s">
         <v>8</v>
@@ -6955,10 +6952,10 @@
         <v>360</v>
       </c>
       <c r="B387" s="12" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C387" s="8" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="D387" s="5" t="s">
         <v>8</v>
@@ -6969,10 +6966,10 @@
         <v>361</v>
       </c>
       <c r="B388" s="12" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C388" s="8" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="D388" s="5" t="s">
         <v>8</v>
@@ -6983,10 +6980,10 @@
         <v>362</v>
       </c>
       <c r="B389" s="12" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C389" s="8" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="D389" s="5" t="s">
         <v>8</v>
@@ -6997,10 +6994,10 @@
         <v>363</v>
       </c>
       <c r="B390" s="12" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C390" s="8" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="D390" s="5" t="s">
         <v>8</v>
@@ -7011,10 +7008,10 @@
         <v>364</v>
       </c>
       <c r="B391" s="12" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C391" s="8" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="D391" s="5" t="s">
         <v>8</v>
@@ -7025,10 +7022,10 @@
         <v>365</v>
       </c>
       <c r="B392" s="12" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C392" s="8" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="D392" s="5" t="s">
         <v>8</v>
@@ -7039,10 +7036,10 @@
         <v>366</v>
       </c>
       <c r="B393" s="12" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C393" s="8" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="D393" s="5" t="s">
         <v>8</v>
@@ -7053,10 +7050,10 @@
         <v>367</v>
       </c>
       <c r="B394" s="12" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C394" s="8" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="D394" s="5" t="s">
         <v>8</v>
@@ -7067,10 +7064,10 @@
         <v>368</v>
       </c>
       <c r="B395" s="12" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C395" s="8" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="D395" s="5" t="s">
         <v>8</v>
@@ -7081,10 +7078,10 @@
         <v>369</v>
       </c>
       <c r="B396" s="12" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C396" s="8" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="D396" s="5" t="s">
         <v>8</v>
@@ -7095,10 +7092,10 @@
         <v>370</v>
       </c>
       <c r="B397" s="12" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C397" s="8" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="D397" s="5" t="s">
         <v>8</v>
@@ -7109,10 +7106,10 @@
         <v>371</v>
       </c>
       <c r="B398" s="12" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C398" s="8" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="D398" s="5" t="s">
         <v>8</v>
@@ -7123,10 +7120,10 @@
         <v>372</v>
       </c>
       <c r="B399" s="12" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C399" s="8" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="D399" s="5" t="s">
         <v>8</v>
@@ -7145,10 +7142,10 @@
         <v>373</v>
       </c>
       <c r="B402" s="12" t="s">
+        <v>388</v>
+      </c>
+      <c r="C402" s="8" t="s">
         <v>389</v>
-      </c>
-      <c r="C402" s="8" t="s">
-        <v>390</v>
       </c>
       <c r="D402" s="5" t="s">
         <v>8</v>
@@ -7159,10 +7156,10 @@
         <v>374</v>
       </c>
       <c r="B403" s="12" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="C403" s="8" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="D403" s="5" t="s">
         <v>8</v>
@@ -7173,10 +7170,10 @@
         <v>375</v>
       </c>
       <c r="B404" s="12" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="C404" s="8" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="D404" s="5" t="s">
         <v>8</v>
@@ -7187,7 +7184,7 @@
         <v>376</v>
       </c>
       <c r="B405" s="12" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="C405" s="8" t="s">
         <v>91</v>
@@ -7201,10 +7198,10 @@
         <v>377</v>
       </c>
       <c r="B406" s="12" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="C406" s="8" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="D406" s="5" t="s">
         <v>8</v>
@@ -7215,10 +7212,10 @@
         <v>378</v>
       </c>
       <c r="B407" s="12" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="C407" s="8" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="D407" s="5" t="s">
         <v>8</v>
@@ -7238,10 +7235,10 @@
         <v>379</v>
       </c>
       <c r="B410" s="7" t="s">
+        <v>394</v>
+      </c>
+      <c r="C410" s="8" t="s">
         <v>395</v>
-      </c>
-      <c r="C410" s="8" t="s">
-        <v>396</v>
       </c>
       <c r="D410" s="5" t="s">
         <v>8</v>
@@ -7252,10 +7249,10 @@
         <v>380</v>
       </c>
       <c r="B411" s="7" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C411" s="8" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="D411" s="5" t="s">
         <v>8</v>
@@ -7266,10 +7263,10 @@
         <v>381</v>
       </c>
       <c r="B412" s="7" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C412" s="8" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="D412" s="5" t="s">
         <v>8</v>
@@ -7280,10 +7277,10 @@
         <v>382</v>
       </c>
       <c r="B413" s="7" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C413" s="8" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="D413" s="5" t="s">
         <v>8</v>
@@ -7294,10 +7291,10 @@
         <v>383</v>
       </c>
       <c r="B414" s="7" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C414" s="8" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="D414" s="5" t="s">
         <v>8</v>
@@ -7308,10 +7305,10 @@
         <v>384</v>
       </c>
       <c r="B415" s="7" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C415" s="8" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="D415" s="5" t="s">
         <v>8</v>
@@ -7322,10 +7319,10 @@
         <v>385</v>
       </c>
       <c r="B416" s="7" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C416" s="8" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="D416" s="5" t="s">
         <v>8</v>
@@ -7336,10 +7333,10 @@
         <v>386</v>
       </c>
       <c r="B417" s="7" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C417" s="8" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D417" s="5" t="s">
         <v>8</v>
@@ -7350,10 +7347,10 @@
         <v>387</v>
       </c>
       <c r="B418" s="7" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C418" s="8" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="D418" s="5" t="s">
         <v>8</v>
@@ -7364,10 +7361,10 @@
         <v>388</v>
       </c>
       <c r="B419" s="7" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C419" s="8" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="D419" s="5" t="s">
         <v>8</v>
@@ -7378,10 +7375,10 @@
         <v>389</v>
       </c>
       <c r="B420" s="7" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C420" s="8" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="D420" s="5" t="s">
         <v>8</v>
@@ -7392,10 +7389,10 @@
         <v>390</v>
       </c>
       <c r="B421" s="7" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C421" s="8" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="D421" s="5" t="s">
         <v>8</v>
@@ -7406,10 +7403,10 @@
         <v>391</v>
       </c>
       <c r="B422" s="7" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C422" s="8" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="D422" s="5" t="s">
         <v>8</v>
@@ -7420,10 +7417,10 @@
         <v>392</v>
       </c>
       <c r="B423" s="7" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C423" s="8" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="D423" s="5" t="s">
         <v>8</v>
@@ -7434,10 +7431,10 @@
         <v>393</v>
       </c>
       <c r="B424" s="7" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C424" s="8" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="D424" s="5" t="s">
         <v>8</v>
@@ -7448,10 +7445,10 @@
         <v>394</v>
       </c>
       <c r="B425" s="7" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C425" s="8" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="D425" s="5" t="s">
         <v>8</v>
@@ -7462,10 +7459,10 @@
         <v>395</v>
       </c>
       <c r="B426" s="7" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C426" s="8" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D426" s="5" t="s">
         <v>8</v>
@@ -7476,10 +7473,10 @@
         <v>396</v>
       </c>
       <c r="B427" s="7" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C427" s="8" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="D427" s="5" t="s">
         <v>8</v>
@@ -7490,10 +7487,10 @@
         <v>397</v>
       </c>
       <c r="B428" s="7" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C428" s="8" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D428" s="5" t="s">
         <v>8</v>
@@ -7504,10 +7501,10 @@
         <v>398</v>
       </c>
       <c r="B429" s="7" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C429" s="8" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="D429" s="5" t="s">
         <v>8</v>
@@ -7518,10 +7515,10 @@
         <v>399</v>
       </c>
       <c r="B430" s="7" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C430" s="8" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="D430" s="5" t="s">
         <v>8</v>
@@ -7532,10 +7529,10 @@
         <v>400</v>
       </c>
       <c r="B431" s="7" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C431" s="8" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="D431" s="5" t="s">
         <v>8</v>
@@ -7546,10 +7543,10 @@
         <v>401</v>
       </c>
       <c r="B432" s="7" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C432" s="8" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="D432" s="5" t="s">
         <v>8</v>
@@ -7560,10 +7557,10 @@
         <v>402</v>
       </c>
       <c r="B433" s="7" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C433" s="8" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="D433" s="5" t="s">
         <v>8</v>
@@ -7574,10 +7571,10 @@
         <v>403</v>
       </c>
       <c r="B434" s="7" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C434" s="8" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D434" s="5" t="s">
         <v>8</v>
@@ -7588,10 +7585,10 @@
         <v>404</v>
       </c>
       <c r="B435" s="7" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C435" s="8" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="D435" s="5" t="s">
         <v>8</v>
@@ -7602,10 +7599,10 @@
         <v>405</v>
       </c>
       <c r="B436" s="7" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C436" s="8" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="D436" s="5" t="s">
         <v>8</v>
@@ -7616,10 +7613,10 @@
         <v>406</v>
       </c>
       <c r="B437" s="7" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C437" s="8" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D437" s="5" t="s">
         <v>8</v>
@@ -7630,10 +7627,10 @@
         <v>407</v>
       </c>
       <c r="B438" s="7" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C438" s="8" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="D438" s="5" t="s">
         <v>8</v>
@@ -7644,10 +7641,10 @@
         <v>408</v>
       </c>
       <c r="B439" s="7" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C439" s="8" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="D439" s="5" t="s">
         <v>8</v>
@@ -7658,10 +7655,10 @@
         <v>409</v>
       </c>
       <c r="B440" s="7" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C440" s="8" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="D440" s="5" t="s">
         <v>8</v>
@@ -7672,10 +7669,10 @@
         <v>410</v>
       </c>
       <c r="B441" s="7" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C441" s="8" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D441" s="5" t="s">
         <v>8</v>
@@ -7686,10 +7683,10 @@
         <v>411</v>
       </c>
       <c r="B442" s="7" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C442" s="8" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D442" s="5" t="s">
         <v>8</v>
@@ -7700,10 +7697,10 @@
         <v>412</v>
       </c>
       <c r="B443" s="7" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C443" s="8" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="D443" s="5" t="s">
         <v>8</v>
@@ -7714,10 +7711,10 @@
         <v>413</v>
       </c>
       <c r="B444" s="7" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C444" s="8" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="D444" s="5" t="s">
         <v>8</v>
@@ -7728,10 +7725,10 @@
         <v>414</v>
       </c>
       <c r="B445" s="7" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C445" s="8" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D445" s="5" t="s">
         <v>8</v>
@@ -7742,10 +7739,10 @@
         <v>415</v>
       </c>
       <c r="B446" s="7" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C446" s="8" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="D446" s="5" t="s">
         <v>8</v>
@@ -7756,10 +7753,10 @@
         <v>416</v>
       </c>
       <c r="B447" s="7" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C447" s="8" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="D447" s="5" t="s">
         <v>8</v>
@@ -7770,10 +7767,10 @@
         <v>417</v>
       </c>
       <c r="B448" s="7" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C448" s="8" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="D448" s="5" t="s">
         <v>8</v>
@@ -7784,10 +7781,10 @@
         <v>418</v>
       </c>
       <c r="B449" s="7" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C449" s="8" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="D449" s="5" t="s">
         <v>8</v>
@@ -7798,10 +7795,10 @@
         <v>419</v>
       </c>
       <c r="B450" s="7" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C450" s="8" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="D450" s="5" t="s">
         <v>8</v>
@@ -7812,10 +7809,10 @@
         <v>420</v>
       </c>
       <c r="B451" s="7" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C451" s="8" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D451" s="5" t="s">
         <v>8</v>
@@ -7826,10 +7823,10 @@
         <v>421</v>
       </c>
       <c r="B452" s="7" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C452" s="8" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="D452" s="5" t="s">
         <v>8</v>
@@ -7840,10 +7837,10 @@
         <v>422</v>
       </c>
       <c r="B453" s="7" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C453" s="8" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="D453" s="5" t="s">
         <v>8</v>
@@ -7854,10 +7851,10 @@
         <v>423</v>
       </c>
       <c r="B454" s="7" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C454" s="8" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="D454" s="5" t="s">
         <v>8</v>
@@ -7868,10 +7865,10 @@
         <v>424</v>
       </c>
       <c r="B455" s="7" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C455" s="8" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="D455" s="5" t="s">
         <v>8</v>
@@ -7882,10 +7879,10 @@
         <v>425</v>
       </c>
       <c r="B456" s="7" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C456" s="8" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="D456" s="5" t="s">
         <v>8</v>
@@ -7896,10 +7893,10 @@
         <v>426</v>
       </c>
       <c r="B457" s="7" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C457" s="8" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="D457" s="5" t="s">
         <v>8</v>
@@ -7910,10 +7907,10 @@
         <v>427</v>
       </c>
       <c r="B458" s="7" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C458" s="8" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="D458" s="5" t="s">
         <v>8</v>
@@ -7924,10 +7921,10 @@
         <v>428</v>
       </c>
       <c r="B459" s="7" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C459" s="8" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="D459" s="5" t="s">
         <v>8</v>
@@ -7938,10 +7935,10 @@
         <v>429</v>
       </c>
       <c r="B460" s="7" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C460" s="8" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="D460" s="5" t="s">
         <v>8</v>
@@ -7952,10 +7949,10 @@
         <v>430</v>
       </c>
       <c r="B461" s="7" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C461" s="8" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="D461" s="5" t="s">
         <v>8</v>
@@ -7966,10 +7963,10 @@
         <v>431</v>
       </c>
       <c r="B462" s="7" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C462" s="8" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="D462" s="5" t="s">
         <v>8</v>
@@ -7980,10 +7977,10 @@
         <v>432</v>
       </c>
       <c r="B463" s="7" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C463" s="8" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="D463" s="5" t="s">
         <v>8</v>
@@ -7994,10 +7991,10 @@
         <v>433</v>
       </c>
       <c r="B464" s="7" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C464" s="8" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D464" s="5" t="s">
         <v>8</v>
@@ -8008,10 +8005,10 @@
         <v>434</v>
       </c>
       <c r="B465" s="7" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C465" s="8" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="D465" s="5" t="s">
         <v>8</v>
@@ -8022,10 +8019,10 @@
         <v>435</v>
       </c>
       <c r="B466" s="7" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C466" s="8" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="D466" s="5" t="s">
         <v>8</v>
@@ -8036,10 +8033,10 @@
         <v>436</v>
       </c>
       <c r="B467" s="7" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C467" s="8" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D467" s="5" t="s">
         <v>8</v>
@@ -8050,10 +8047,10 @@
         <v>437</v>
       </c>
       <c r="B468" s="7" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C468" s="8" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="D468" s="5" t="s">
         <v>8</v>
@@ -8064,10 +8061,10 @@
         <v>438</v>
       </c>
       <c r="B469" s="7" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C469" s="8" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="D469" s="5" t="s">
         <v>8</v>
@@ -8087,10 +8084,10 @@
         <v>439</v>
       </c>
       <c r="B472" s="7" t="s">
+        <v>454</v>
+      </c>
+      <c r="C472" s="8" t="s">
         <v>455</v>
-      </c>
-      <c r="C472" s="8" t="s">
-        <v>456</v>
       </c>
       <c r="D472" s="5" t="s">
         <v>8</v>
@@ -8101,10 +8098,10 @@
         <v>440</v>
       </c>
       <c r="B473" s="7" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="C473" s="8" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="D473" s="5" t="s">
         <v>8</v>
@@ -8115,10 +8112,10 @@
         <v>441</v>
       </c>
       <c r="B474" s="7" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="C474" s="8" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="D474" s="5" t="s">
         <v>8</v>
@@ -8129,10 +8126,10 @@
         <v>442</v>
       </c>
       <c r="B475" s="7" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="C475" s="8" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="D475" s="5" t="s">
         <v>8</v>
@@ -8143,10 +8140,10 @@
         <v>443</v>
       </c>
       <c r="B476" s="7" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="C476" s="8" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="D476" s="5" t="s">
         <v>8</v>
@@ -8157,10 +8154,10 @@
         <v>444</v>
       </c>
       <c r="B477" s="7" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="C477" s="8" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="D477" s="5" t="s">
         <v>8</v>
@@ -8171,10 +8168,10 @@
         <v>445</v>
       </c>
       <c r="B478" s="7" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="C478" s="8" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="D478" s="5" t="s">
         <v>8</v>
@@ -8185,10 +8182,10 @@
         <v>446</v>
       </c>
       <c r="B479" s="7" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="C479" s="8" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="D479" s="5" t="s">
         <v>8</v>
@@ -8199,10 +8196,10 @@
         <v>447</v>
       </c>
       <c r="B480" s="7" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="C480" s="8" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="D480" s="5" t="s">
         <v>8</v>
@@ -8213,10 +8210,10 @@
         <v>448</v>
       </c>
       <c r="B481" s="7" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="C481" s="8" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="D481" s="5" t="s">
         <v>8</v>
@@ -8350,326 +8347,326 @@
     <hyperlink ref="C135" r:id="rId124" xr:uid="{00000000-0004-0000-0000-00007B000000}"/>
     <hyperlink ref="C136" r:id="rId125" xr:uid="{00000000-0004-0000-0000-00007C000000}"/>
     <hyperlink ref="C139" r:id="rId126" xr:uid="{00000000-0004-0000-0000-00007D000000}"/>
-    <hyperlink ref="C140" r:id="rId127" xr:uid="{00000000-0004-0000-0000-00007E000000}"/>
-    <hyperlink ref="C141" r:id="rId128" xr:uid="{00000000-0004-0000-0000-00007F000000}"/>
-    <hyperlink ref="C142" r:id="rId129" xr:uid="{00000000-0004-0000-0000-000080000000}"/>
-    <hyperlink ref="C143" r:id="rId130" xr:uid="{00000000-0004-0000-0000-000081000000}"/>
-    <hyperlink ref="C144" r:id="rId131" xr:uid="{00000000-0004-0000-0000-000082000000}"/>
-    <hyperlink ref="C145" r:id="rId132" xr:uid="{00000000-0004-0000-0000-000083000000}"/>
-    <hyperlink ref="C146" r:id="rId133" xr:uid="{00000000-0004-0000-0000-000084000000}"/>
-    <hyperlink ref="C147" r:id="rId134" xr:uid="{00000000-0004-0000-0000-000085000000}"/>
-    <hyperlink ref="C148" r:id="rId135" xr:uid="{00000000-0004-0000-0000-000086000000}"/>
-    <hyperlink ref="C149" r:id="rId136" xr:uid="{00000000-0004-0000-0000-000087000000}"/>
-    <hyperlink ref="C150" r:id="rId137" xr:uid="{00000000-0004-0000-0000-000088000000}"/>
-    <hyperlink ref="C151" r:id="rId138" xr:uid="{00000000-0004-0000-0000-000089000000}"/>
-    <hyperlink ref="C152" r:id="rId139" xr:uid="{00000000-0004-0000-0000-00008A000000}"/>
-    <hyperlink ref="C153" r:id="rId140" xr:uid="{00000000-0004-0000-0000-00008B000000}"/>
-    <hyperlink ref="C154" r:id="rId141" xr:uid="{00000000-0004-0000-0000-00008C000000}"/>
-    <hyperlink ref="C155" r:id="rId142" xr:uid="{00000000-0004-0000-0000-00008D000000}"/>
-    <hyperlink ref="C156" r:id="rId143" xr:uid="{00000000-0004-0000-0000-00008E000000}"/>
-    <hyperlink ref="C157" r:id="rId144" xr:uid="{00000000-0004-0000-0000-00008F000000}"/>
-    <hyperlink ref="C158" r:id="rId145" xr:uid="{00000000-0004-0000-0000-000090000000}"/>
-    <hyperlink ref="C159" r:id="rId146" xr:uid="{00000000-0004-0000-0000-000091000000}"/>
-    <hyperlink ref="C160" r:id="rId147" xr:uid="{00000000-0004-0000-0000-000092000000}"/>
-    <hyperlink ref="C161" r:id="rId148" xr:uid="{00000000-0004-0000-0000-000093000000}"/>
-    <hyperlink ref="C162" r:id="rId149" xr:uid="{00000000-0004-0000-0000-000094000000}"/>
-    <hyperlink ref="C163" r:id="rId150" xr:uid="{00000000-0004-0000-0000-000095000000}"/>
-    <hyperlink ref="C166" r:id="rId151" xr:uid="{00000000-0004-0000-0000-000096000000}"/>
-    <hyperlink ref="C167" r:id="rId152" xr:uid="{00000000-0004-0000-0000-000097000000}"/>
-    <hyperlink ref="C168" r:id="rId153" xr:uid="{00000000-0004-0000-0000-000098000000}"/>
-    <hyperlink ref="C169" r:id="rId154" xr:uid="{00000000-0004-0000-0000-000099000000}"/>
-    <hyperlink ref="C170" r:id="rId155" xr:uid="{00000000-0004-0000-0000-00009A000000}"/>
-    <hyperlink ref="C171" r:id="rId156" xr:uid="{00000000-0004-0000-0000-00009B000000}"/>
-    <hyperlink ref="C172" r:id="rId157" xr:uid="{00000000-0004-0000-0000-00009C000000}"/>
-    <hyperlink ref="C173" r:id="rId158" xr:uid="{00000000-0004-0000-0000-00009D000000}"/>
-    <hyperlink ref="C174" r:id="rId159" xr:uid="{00000000-0004-0000-0000-00009E000000}"/>
-    <hyperlink ref="C177" r:id="rId160" xr:uid="{00000000-0004-0000-0000-00009F000000}"/>
-    <hyperlink ref="C178" r:id="rId161" xr:uid="{00000000-0004-0000-0000-0000A0000000}"/>
-    <hyperlink ref="C179" r:id="rId162" xr:uid="{00000000-0004-0000-0000-0000A1000000}"/>
-    <hyperlink ref="C180" r:id="rId163" xr:uid="{00000000-0004-0000-0000-0000A2000000}"/>
-    <hyperlink ref="C181" r:id="rId164" xr:uid="{00000000-0004-0000-0000-0000A3000000}"/>
-    <hyperlink ref="C182" r:id="rId165" xr:uid="{00000000-0004-0000-0000-0000A4000000}"/>
-    <hyperlink ref="C183" r:id="rId166" xr:uid="{00000000-0004-0000-0000-0000A5000000}"/>
-    <hyperlink ref="C184" r:id="rId167" xr:uid="{00000000-0004-0000-0000-0000A6000000}"/>
-    <hyperlink ref="C185" r:id="rId168" xr:uid="{00000000-0004-0000-0000-0000A7000000}"/>
-    <hyperlink ref="C186" r:id="rId169" xr:uid="{00000000-0004-0000-0000-0000A8000000}"/>
-    <hyperlink ref="C187" r:id="rId170" xr:uid="{00000000-0004-0000-0000-0000A9000000}"/>
-    <hyperlink ref="C188" r:id="rId171" xr:uid="{00000000-0004-0000-0000-0000AA000000}"/>
-    <hyperlink ref="C189" r:id="rId172" xr:uid="{00000000-0004-0000-0000-0000AB000000}"/>
-    <hyperlink ref="C190" r:id="rId173" xr:uid="{00000000-0004-0000-0000-0000AC000000}"/>
-    <hyperlink ref="C191" r:id="rId174" xr:uid="{00000000-0004-0000-0000-0000AD000000}"/>
-    <hyperlink ref="C192" r:id="rId175" xr:uid="{00000000-0004-0000-0000-0000AE000000}"/>
-    <hyperlink ref="C193" r:id="rId176" xr:uid="{00000000-0004-0000-0000-0000AF000000}"/>
-    <hyperlink ref="C194" r:id="rId177" xr:uid="{00000000-0004-0000-0000-0000B0000000}"/>
-    <hyperlink ref="C195" r:id="rId178" xr:uid="{00000000-0004-0000-0000-0000B1000000}"/>
-    <hyperlink ref="C196" r:id="rId179" xr:uid="{00000000-0004-0000-0000-0000B2000000}"/>
-    <hyperlink ref="C197" r:id="rId180" location=":~:text=Given%20the%20array%20representation%20of,it%20into%20Binary%20Search%20Tree.&amp;text=Swap%201%3A%20Swap%20node%208,node%209%20with%20node%2010." xr:uid="{00000000-0004-0000-0000-0000B3000000}"/>
-    <hyperlink ref="C198" r:id="rId181" xr:uid="{00000000-0004-0000-0000-0000B4000000}"/>
-    <hyperlink ref="C199" r:id="rId182" xr:uid="{00000000-0004-0000-0000-0000B5000000}"/>
-    <hyperlink ref="C200" r:id="rId183" xr:uid="{00000000-0004-0000-0000-0000B6000000}"/>
-    <hyperlink ref="C201" r:id="rId184" xr:uid="{00000000-0004-0000-0000-0000B7000000}"/>
-    <hyperlink ref="C202" r:id="rId185" xr:uid="{00000000-0004-0000-0000-0000B8000000}"/>
-    <hyperlink ref="C203" r:id="rId186" location=":~:text=Since%20the%20graph%20is%20undirected,graph%20is%20connected%2C%20otherwise%20not." xr:uid="{00000000-0004-0000-0000-0000B9000000}"/>
-    <hyperlink ref="C204" r:id="rId187" xr:uid="{00000000-0004-0000-0000-0000BA000000}"/>
-    <hyperlink ref="C205" r:id="rId188" xr:uid="{00000000-0004-0000-0000-0000BB000000}"/>
-    <hyperlink ref="C206" r:id="rId189" xr:uid="{00000000-0004-0000-0000-0000BC000000}"/>
-    <hyperlink ref="C207" r:id="rId190" xr:uid="{00000000-0004-0000-0000-0000BD000000}"/>
-    <hyperlink ref="C208" r:id="rId191" xr:uid="{00000000-0004-0000-0000-0000BE000000}"/>
-    <hyperlink ref="C209" r:id="rId192" xr:uid="{00000000-0004-0000-0000-0000BF000000}"/>
-    <hyperlink ref="C210" r:id="rId193" xr:uid="{00000000-0004-0000-0000-0000C0000000}"/>
-    <hyperlink ref="C211" r:id="rId194" xr:uid="{00000000-0004-0000-0000-0000C1000000}"/>
-    <hyperlink ref="C214" r:id="rId195" xr:uid="{00000000-0004-0000-0000-0000C2000000}"/>
-    <hyperlink ref="C215" r:id="rId196" xr:uid="{00000000-0004-0000-0000-0000C3000000}"/>
-    <hyperlink ref="C216" r:id="rId197" xr:uid="{00000000-0004-0000-0000-0000C4000000}"/>
-    <hyperlink ref="C217" r:id="rId198" xr:uid="{00000000-0004-0000-0000-0000C5000000}"/>
-    <hyperlink ref="C218" r:id="rId199" xr:uid="{00000000-0004-0000-0000-0000C6000000}"/>
-    <hyperlink ref="C219" r:id="rId200" xr:uid="{00000000-0004-0000-0000-0000C7000000}"/>
-    <hyperlink ref="C220" r:id="rId201" xr:uid="{00000000-0004-0000-0000-0000C8000000}"/>
-    <hyperlink ref="C221" r:id="rId202" xr:uid="{00000000-0004-0000-0000-0000C9000000}"/>
-    <hyperlink ref="C222" r:id="rId203" xr:uid="{00000000-0004-0000-0000-0000CA000000}"/>
-    <hyperlink ref="C223" r:id="rId204" xr:uid="{00000000-0004-0000-0000-0000CB000000}"/>
-    <hyperlink ref="C224" r:id="rId205" xr:uid="{00000000-0004-0000-0000-0000CC000000}"/>
-    <hyperlink ref="C225" r:id="rId206" xr:uid="{00000000-0004-0000-0000-0000CD000000}"/>
-    <hyperlink ref="C226" r:id="rId207" xr:uid="{00000000-0004-0000-0000-0000CE000000}"/>
-    <hyperlink ref="C227" r:id="rId208" xr:uid="{00000000-0004-0000-0000-0000CF000000}"/>
-    <hyperlink ref="C228" r:id="rId209" xr:uid="{00000000-0004-0000-0000-0000D0000000}"/>
-    <hyperlink ref="C229" r:id="rId210" xr:uid="{00000000-0004-0000-0000-0000D1000000}"/>
-    <hyperlink ref="C230" r:id="rId211" xr:uid="{00000000-0004-0000-0000-0000D2000000}"/>
-    <hyperlink ref="C231" r:id="rId212" xr:uid="{00000000-0004-0000-0000-0000D3000000}"/>
-    <hyperlink ref="C232" r:id="rId213" xr:uid="{00000000-0004-0000-0000-0000D4000000}"/>
-    <hyperlink ref="C233" r:id="rId214" xr:uid="{00000000-0004-0000-0000-0000D5000000}"/>
-    <hyperlink ref="C234" r:id="rId215" xr:uid="{00000000-0004-0000-0000-0000D6000000}"/>
-    <hyperlink ref="C235" r:id="rId216" xr:uid="{00000000-0004-0000-0000-0000D7000000}"/>
-    <hyperlink ref="C238" r:id="rId217" xr:uid="{00000000-0004-0000-0000-0000D8000000}"/>
-    <hyperlink ref="C239" r:id="rId218" xr:uid="{00000000-0004-0000-0000-0000D9000000}"/>
-    <hyperlink ref="C240" r:id="rId219" xr:uid="{00000000-0004-0000-0000-0000DA000000}"/>
-    <hyperlink ref="C241" r:id="rId220" xr:uid="{00000000-0004-0000-0000-0000DB000000}"/>
-    <hyperlink ref="C242" r:id="rId221" xr:uid="{00000000-0004-0000-0000-0000DC000000}"/>
-    <hyperlink ref="C243" r:id="rId222" xr:uid="{00000000-0004-0000-0000-0000DD000000}"/>
-    <hyperlink ref="C244" r:id="rId223" xr:uid="{00000000-0004-0000-0000-0000DE000000}"/>
-    <hyperlink ref="C245" r:id="rId224" xr:uid="{00000000-0004-0000-0000-0000DF000000}"/>
-    <hyperlink ref="C246" r:id="rId225" xr:uid="{00000000-0004-0000-0000-0000E0000000}"/>
-    <hyperlink ref="C247" r:id="rId226" xr:uid="{00000000-0004-0000-0000-0000E1000000}"/>
-    <hyperlink ref="C248" r:id="rId227" xr:uid="{00000000-0004-0000-0000-0000E2000000}"/>
-    <hyperlink ref="C249" r:id="rId228" xr:uid="{00000000-0004-0000-0000-0000E3000000}"/>
-    <hyperlink ref="C250" r:id="rId229" xr:uid="{00000000-0004-0000-0000-0000E4000000}"/>
-    <hyperlink ref="C251" r:id="rId230" xr:uid="{00000000-0004-0000-0000-0000E5000000}"/>
-    <hyperlink ref="C252" r:id="rId231" xr:uid="{00000000-0004-0000-0000-0000E6000000}"/>
-    <hyperlink ref="C253" r:id="rId232" xr:uid="{00000000-0004-0000-0000-0000E7000000}"/>
-    <hyperlink ref="C254" r:id="rId233" xr:uid="{00000000-0004-0000-0000-0000E8000000}"/>
-    <hyperlink ref="C255" r:id="rId234" xr:uid="{00000000-0004-0000-0000-0000E9000000}"/>
-    <hyperlink ref="C256" r:id="rId235" xr:uid="{00000000-0004-0000-0000-0000EA000000}"/>
-    <hyperlink ref="C257" r:id="rId236" location=":~:text=It%20consists%20of%20two%20steps,result%20to%20the%20sum%20S." xr:uid="{00000000-0004-0000-0000-0000EB000000}"/>
-    <hyperlink ref="C258" r:id="rId237" xr:uid="{00000000-0004-0000-0000-0000EC000000}"/>
-    <hyperlink ref="C259" r:id="rId238" xr:uid="{00000000-0004-0000-0000-0000ED000000}"/>
-    <hyperlink ref="C260" r:id="rId239" xr:uid="{00000000-0004-0000-0000-0000EE000000}"/>
-    <hyperlink ref="C261" r:id="rId240" xr:uid="{00000000-0004-0000-0000-0000EF000000}"/>
-    <hyperlink ref="C262" r:id="rId241" xr:uid="{00000000-0004-0000-0000-0000F0000000}"/>
-    <hyperlink ref="C263" r:id="rId242" xr:uid="{00000000-0004-0000-0000-0000F1000000}"/>
-    <hyperlink ref="C264" r:id="rId243" xr:uid="{00000000-0004-0000-0000-0000F2000000}"/>
-    <hyperlink ref="C265" r:id="rId244" xr:uid="{00000000-0004-0000-0000-0000F3000000}"/>
-    <hyperlink ref="C266" r:id="rId245" xr:uid="{00000000-0004-0000-0000-0000F4000000}"/>
-    <hyperlink ref="C267" r:id="rId246" xr:uid="{00000000-0004-0000-0000-0000F5000000}"/>
-    <hyperlink ref="C268" r:id="rId247" xr:uid="{00000000-0004-0000-0000-0000F6000000}"/>
-    <hyperlink ref="C269" r:id="rId248" xr:uid="{00000000-0004-0000-0000-0000F7000000}"/>
-    <hyperlink ref="C270" r:id="rId249" xr:uid="{00000000-0004-0000-0000-0000F8000000}"/>
-    <hyperlink ref="C271" r:id="rId250" xr:uid="{00000000-0004-0000-0000-0000F9000000}"/>
-    <hyperlink ref="C272" r:id="rId251" xr:uid="{00000000-0004-0000-0000-0000FA000000}"/>
-    <hyperlink ref="C275" r:id="rId252" xr:uid="{00000000-0004-0000-0000-0000FB000000}"/>
-    <hyperlink ref="C276" r:id="rId253" xr:uid="{00000000-0004-0000-0000-0000FC000000}"/>
-    <hyperlink ref="C277" r:id="rId254" xr:uid="{00000000-0004-0000-0000-0000FD000000}"/>
-    <hyperlink ref="C278" r:id="rId255" xr:uid="{00000000-0004-0000-0000-0000FE000000}"/>
-    <hyperlink ref="C279" r:id="rId256" xr:uid="{00000000-0004-0000-0000-0000FF000000}"/>
-    <hyperlink ref="C280" r:id="rId257" xr:uid="{00000000-0004-0000-0000-000000010000}"/>
-    <hyperlink ref="C281" r:id="rId258" xr:uid="{00000000-0004-0000-0000-000001010000}"/>
-    <hyperlink ref="C282" r:id="rId259" xr:uid="{00000000-0004-0000-0000-000002010000}"/>
-    <hyperlink ref="C283" r:id="rId260" xr:uid="{00000000-0004-0000-0000-000003010000}"/>
-    <hyperlink ref="C284" r:id="rId261" xr:uid="{00000000-0004-0000-0000-000004010000}"/>
-    <hyperlink ref="C285" r:id="rId262" xr:uid="{00000000-0004-0000-0000-000005010000}"/>
-    <hyperlink ref="C286" r:id="rId263" xr:uid="{00000000-0004-0000-0000-000006010000}"/>
-    <hyperlink ref="C287" r:id="rId264" xr:uid="{00000000-0004-0000-0000-000007010000}"/>
-    <hyperlink ref="C288" r:id="rId265" xr:uid="{00000000-0004-0000-0000-000008010000}"/>
-    <hyperlink ref="C289" r:id="rId266" xr:uid="{00000000-0004-0000-0000-000009010000}"/>
-    <hyperlink ref="C290" r:id="rId267" xr:uid="{00000000-0004-0000-0000-00000A010000}"/>
-    <hyperlink ref="C291" r:id="rId268" xr:uid="{00000000-0004-0000-0000-00000B010000}"/>
-    <hyperlink ref="C292" r:id="rId269" xr:uid="{00000000-0004-0000-0000-00000C010000}"/>
-    <hyperlink ref="C293" r:id="rId270" xr:uid="{00000000-0004-0000-0000-00000D010000}"/>
-    <hyperlink ref="C296" r:id="rId271" xr:uid="{00000000-0004-0000-0000-00000E010000}"/>
-    <hyperlink ref="C297" r:id="rId272" xr:uid="{00000000-0004-0000-0000-00000F010000}"/>
-    <hyperlink ref="C298" r:id="rId273" xr:uid="{00000000-0004-0000-0000-000010010000}"/>
-    <hyperlink ref="C299" r:id="rId274" xr:uid="{00000000-0004-0000-0000-000011010000}"/>
-    <hyperlink ref="C300" r:id="rId275" xr:uid="{00000000-0004-0000-0000-000012010000}"/>
-    <hyperlink ref="C301" r:id="rId276" xr:uid="{00000000-0004-0000-0000-000013010000}"/>
-    <hyperlink ref="C302" r:id="rId277" xr:uid="{00000000-0004-0000-0000-000014010000}"/>
-    <hyperlink ref="C303" r:id="rId278" xr:uid="{00000000-0004-0000-0000-000015010000}"/>
-    <hyperlink ref="C304" r:id="rId279" xr:uid="{00000000-0004-0000-0000-000016010000}"/>
-    <hyperlink ref="C305" r:id="rId280" xr:uid="{00000000-0004-0000-0000-000017010000}"/>
-    <hyperlink ref="C306" r:id="rId281" location=":~:text=The%20stack%20organization%20is%20very,i.e.%2C%20A%20%2B%20B)." xr:uid="{00000000-0004-0000-0000-000018010000}"/>
-    <hyperlink ref="C307" r:id="rId282" xr:uid="{00000000-0004-0000-0000-000019010000}"/>
-    <hyperlink ref="C308" r:id="rId283" xr:uid="{00000000-0004-0000-0000-00001A010000}"/>
-    <hyperlink ref="C309" r:id="rId284" xr:uid="{00000000-0004-0000-0000-00001B010000}"/>
-    <hyperlink ref="C310" r:id="rId285" xr:uid="{00000000-0004-0000-0000-00001C010000}"/>
-    <hyperlink ref="C311" r:id="rId286" xr:uid="{00000000-0004-0000-0000-00001D010000}"/>
-    <hyperlink ref="C312" r:id="rId287" xr:uid="{00000000-0004-0000-0000-00001E010000}"/>
-    <hyperlink ref="C313" r:id="rId288" xr:uid="{00000000-0004-0000-0000-00001F010000}"/>
-    <hyperlink ref="C314" r:id="rId289" xr:uid="{00000000-0004-0000-0000-000020010000}"/>
-    <hyperlink ref="C315" r:id="rId290" xr:uid="{00000000-0004-0000-0000-000021010000}"/>
-    <hyperlink ref="C316" r:id="rId291" xr:uid="{00000000-0004-0000-0000-000022010000}"/>
-    <hyperlink ref="C317" r:id="rId292" xr:uid="{00000000-0004-0000-0000-000023010000}"/>
-    <hyperlink ref="C318" r:id="rId293" xr:uid="{00000000-0004-0000-0000-000024010000}"/>
-    <hyperlink ref="C319" r:id="rId294" xr:uid="{00000000-0004-0000-0000-000025010000}"/>
-    <hyperlink ref="C320" r:id="rId295" xr:uid="{00000000-0004-0000-0000-000026010000}"/>
-    <hyperlink ref="C321" r:id="rId296" xr:uid="{00000000-0004-0000-0000-000027010000}"/>
-    <hyperlink ref="C322" r:id="rId297" xr:uid="{00000000-0004-0000-0000-000028010000}"/>
-    <hyperlink ref="C323" r:id="rId298" xr:uid="{00000000-0004-0000-0000-000029010000}"/>
-    <hyperlink ref="C324" r:id="rId299" xr:uid="{00000000-0004-0000-0000-00002A010000}"/>
-    <hyperlink ref="C325" r:id="rId300" xr:uid="{00000000-0004-0000-0000-00002B010000}"/>
-    <hyperlink ref="C326" r:id="rId301" xr:uid="{00000000-0004-0000-0000-00002C010000}"/>
-    <hyperlink ref="C327" r:id="rId302" xr:uid="{00000000-0004-0000-0000-00002D010000}"/>
-    <hyperlink ref="C328" r:id="rId303" xr:uid="{00000000-0004-0000-0000-00002E010000}"/>
-    <hyperlink ref="C329" r:id="rId304" xr:uid="{00000000-0004-0000-0000-00002F010000}"/>
-    <hyperlink ref="C330" r:id="rId305" xr:uid="{00000000-0004-0000-0000-000030010000}"/>
-    <hyperlink ref="C331" r:id="rId306" xr:uid="{00000000-0004-0000-0000-000031010000}"/>
-    <hyperlink ref="C332" r:id="rId307" xr:uid="{00000000-0004-0000-0000-000032010000}"/>
-    <hyperlink ref="C333" r:id="rId308" xr:uid="{00000000-0004-0000-0000-000033010000}"/>
-    <hyperlink ref="C336" r:id="rId309" xr:uid="{00000000-0004-0000-0000-000034010000}"/>
-    <hyperlink ref="C337" r:id="rId310" xr:uid="{00000000-0004-0000-0000-000035010000}"/>
-    <hyperlink ref="C338" r:id="rId311" xr:uid="{00000000-0004-0000-0000-000036010000}"/>
-    <hyperlink ref="C339" r:id="rId312" xr:uid="{00000000-0004-0000-0000-000037010000}"/>
-    <hyperlink ref="C340" r:id="rId313" xr:uid="{00000000-0004-0000-0000-000038010000}"/>
-    <hyperlink ref="C341" r:id="rId314" xr:uid="{00000000-0004-0000-0000-000039010000}"/>
-    <hyperlink ref="C342" r:id="rId315" xr:uid="{00000000-0004-0000-0000-00003A010000}"/>
-    <hyperlink ref="C343" r:id="rId316" xr:uid="{00000000-0004-0000-0000-00003B010000}"/>
-    <hyperlink ref="C344" r:id="rId317" xr:uid="{00000000-0004-0000-0000-00003C010000}"/>
-    <hyperlink ref="C345" r:id="rId318" xr:uid="{00000000-0004-0000-0000-00003D010000}"/>
-    <hyperlink ref="C346" r:id="rId319" xr:uid="{00000000-0004-0000-0000-00003E010000}"/>
-    <hyperlink ref="C347" r:id="rId320" xr:uid="{00000000-0004-0000-0000-00003F010000}"/>
-    <hyperlink ref="C348" r:id="rId321" xr:uid="{00000000-0004-0000-0000-000040010000}"/>
-    <hyperlink ref="C349" r:id="rId322" xr:uid="{00000000-0004-0000-0000-000041010000}"/>
-    <hyperlink ref="C350" r:id="rId323" xr:uid="{00000000-0004-0000-0000-000042010000}"/>
-    <hyperlink ref="C351" r:id="rId324" xr:uid="{00000000-0004-0000-0000-000043010000}"/>
-    <hyperlink ref="C352" r:id="rId325" xr:uid="{00000000-0004-0000-0000-000044010000}"/>
-    <hyperlink ref="C353" r:id="rId326" xr:uid="{00000000-0004-0000-0000-000045010000}"/>
-    <hyperlink ref="C356" r:id="rId327" xr:uid="{00000000-0004-0000-0000-000046010000}"/>
-    <hyperlink ref="C357" r:id="rId328" xr:uid="{00000000-0004-0000-0000-000047010000}"/>
-    <hyperlink ref="C358" r:id="rId329" xr:uid="{00000000-0004-0000-0000-000048010000}"/>
-    <hyperlink ref="C359" r:id="rId330" xr:uid="{00000000-0004-0000-0000-000049010000}"/>
-    <hyperlink ref="C360" r:id="rId331" xr:uid="{00000000-0004-0000-0000-00004A010000}"/>
-    <hyperlink ref="C361" r:id="rId332" xr:uid="{00000000-0004-0000-0000-00004B010000}"/>
-    <hyperlink ref="C362" r:id="rId333" xr:uid="{00000000-0004-0000-0000-00004C010000}"/>
-    <hyperlink ref="C363" r:id="rId334" xr:uid="{00000000-0004-0000-0000-00004D010000}"/>
-    <hyperlink ref="C364" r:id="rId335" xr:uid="{00000000-0004-0000-0000-00004E010000}"/>
-    <hyperlink ref="C365" r:id="rId336" xr:uid="{00000000-0004-0000-0000-00004F010000}"/>
-    <hyperlink ref="C366" r:id="rId337" xr:uid="{00000000-0004-0000-0000-000050010000}"/>
-    <hyperlink ref="C367" r:id="rId338" xr:uid="{00000000-0004-0000-0000-000051010000}"/>
-    <hyperlink ref="C368" r:id="rId339" xr:uid="{00000000-0004-0000-0000-000052010000}"/>
-    <hyperlink ref="C369" r:id="rId340" xr:uid="{00000000-0004-0000-0000-000053010000}"/>
-    <hyperlink ref="C370" r:id="rId341" xr:uid="{00000000-0004-0000-0000-000054010000}"/>
-    <hyperlink ref="C371" r:id="rId342" xr:uid="{00000000-0004-0000-0000-000055010000}"/>
-    <hyperlink ref="C372" r:id="rId343" xr:uid="{00000000-0004-0000-0000-000056010000}"/>
-    <hyperlink ref="C373" r:id="rId344" xr:uid="{00000000-0004-0000-0000-000057010000}"/>
-    <hyperlink ref="C374" r:id="rId345" xr:uid="{00000000-0004-0000-0000-000058010000}"/>
-    <hyperlink ref="C375" r:id="rId346" xr:uid="{00000000-0004-0000-0000-000059010000}"/>
-    <hyperlink ref="C376" r:id="rId347" xr:uid="{00000000-0004-0000-0000-00005A010000}"/>
-    <hyperlink ref="C377" r:id="rId348" xr:uid="{00000000-0004-0000-0000-00005B010000}"/>
-    <hyperlink ref="C378" r:id="rId349" xr:uid="{00000000-0004-0000-0000-00005C010000}"/>
-    <hyperlink ref="C379" r:id="rId350" location=":~:text=Graph%20coloring%20problem%20is%20to,are%20colored%20using%20same%20color." xr:uid="{00000000-0004-0000-0000-00005D010000}"/>
-    <hyperlink ref="C380" r:id="rId351" xr:uid="{00000000-0004-0000-0000-00005E010000}"/>
-    <hyperlink ref="C381" r:id="rId352" xr:uid="{00000000-0004-0000-0000-00005F010000}"/>
-    <hyperlink ref="C382" r:id="rId353" xr:uid="{00000000-0004-0000-0000-000060010000}"/>
-    <hyperlink ref="C383" r:id="rId354" xr:uid="{00000000-0004-0000-0000-000061010000}"/>
-    <hyperlink ref="C384" r:id="rId355" xr:uid="{00000000-0004-0000-0000-000062010000}"/>
-    <hyperlink ref="C385" r:id="rId356" xr:uid="{00000000-0004-0000-0000-000063010000}"/>
-    <hyperlink ref="C386" r:id="rId357" xr:uid="{00000000-0004-0000-0000-000064010000}"/>
-    <hyperlink ref="C387" r:id="rId358" xr:uid="{00000000-0004-0000-0000-000065010000}"/>
-    <hyperlink ref="C388" r:id="rId359" xr:uid="{00000000-0004-0000-0000-000066010000}"/>
-    <hyperlink ref="C389" r:id="rId360" xr:uid="{00000000-0004-0000-0000-000067010000}"/>
-    <hyperlink ref="C390" r:id="rId361" xr:uid="{00000000-0004-0000-0000-000068010000}"/>
-    <hyperlink ref="C391" r:id="rId362" xr:uid="{00000000-0004-0000-0000-000069010000}"/>
-    <hyperlink ref="C392" r:id="rId363" xr:uid="{00000000-0004-0000-0000-00006A010000}"/>
-    <hyperlink ref="C393" r:id="rId364" xr:uid="{00000000-0004-0000-0000-00006B010000}"/>
-    <hyperlink ref="C394" r:id="rId365" xr:uid="{00000000-0004-0000-0000-00006C010000}"/>
-    <hyperlink ref="C395" r:id="rId366" xr:uid="{00000000-0004-0000-0000-00006D010000}"/>
-    <hyperlink ref="C396" r:id="rId367" xr:uid="{00000000-0004-0000-0000-00006E010000}"/>
-    <hyperlink ref="C397" r:id="rId368" xr:uid="{00000000-0004-0000-0000-00006F010000}"/>
-    <hyperlink ref="C398" r:id="rId369" xr:uid="{00000000-0004-0000-0000-000070010000}"/>
-    <hyperlink ref="C399" r:id="rId370" xr:uid="{00000000-0004-0000-0000-000071010000}"/>
-    <hyperlink ref="C402" r:id="rId371" xr:uid="{00000000-0004-0000-0000-000072010000}"/>
-    <hyperlink ref="C403" r:id="rId372" xr:uid="{00000000-0004-0000-0000-000073010000}"/>
-    <hyperlink ref="C404" r:id="rId373" xr:uid="{00000000-0004-0000-0000-000074010000}"/>
-    <hyperlink ref="C405" r:id="rId374" xr:uid="{00000000-0004-0000-0000-000075010000}"/>
-    <hyperlink ref="C406" r:id="rId375" xr:uid="{00000000-0004-0000-0000-000076010000}"/>
-    <hyperlink ref="C407" r:id="rId376" xr:uid="{00000000-0004-0000-0000-000077010000}"/>
-    <hyperlink ref="C410" r:id="rId377" xr:uid="{00000000-0004-0000-0000-000078010000}"/>
-    <hyperlink ref="C411" r:id="rId378" xr:uid="{00000000-0004-0000-0000-000079010000}"/>
-    <hyperlink ref="C412" r:id="rId379" xr:uid="{00000000-0004-0000-0000-00007A010000}"/>
-    <hyperlink ref="C413" r:id="rId380" xr:uid="{00000000-0004-0000-0000-00007B010000}"/>
-    <hyperlink ref="C414" r:id="rId381" xr:uid="{00000000-0004-0000-0000-00007C010000}"/>
-    <hyperlink ref="C415" r:id="rId382" xr:uid="{00000000-0004-0000-0000-00007D010000}"/>
-    <hyperlink ref="C416" r:id="rId383" xr:uid="{00000000-0004-0000-0000-00007E010000}"/>
-    <hyperlink ref="C417" r:id="rId384" xr:uid="{00000000-0004-0000-0000-00007F010000}"/>
-    <hyperlink ref="C418" r:id="rId385" xr:uid="{00000000-0004-0000-0000-000080010000}"/>
-    <hyperlink ref="C419" r:id="rId386" xr:uid="{00000000-0004-0000-0000-000081010000}"/>
-    <hyperlink ref="C420" r:id="rId387" xr:uid="{00000000-0004-0000-0000-000082010000}"/>
-    <hyperlink ref="C421" r:id="rId388" xr:uid="{00000000-0004-0000-0000-000083010000}"/>
-    <hyperlink ref="C422" r:id="rId389" xr:uid="{00000000-0004-0000-0000-000084010000}"/>
-    <hyperlink ref="C423" r:id="rId390" xr:uid="{00000000-0004-0000-0000-000085010000}"/>
-    <hyperlink ref="C424" r:id="rId391" xr:uid="{00000000-0004-0000-0000-000086010000}"/>
-    <hyperlink ref="C425" r:id="rId392" xr:uid="{00000000-0004-0000-0000-000087010000}"/>
-    <hyperlink ref="C426" r:id="rId393" xr:uid="{00000000-0004-0000-0000-000088010000}"/>
-    <hyperlink ref="C427" r:id="rId394" xr:uid="{00000000-0004-0000-0000-000089010000}"/>
-    <hyperlink ref="C428" r:id="rId395" xr:uid="{00000000-0004-0000-0000-00008A010000}"/>
-    <hyperlink ref="C429" r:id="rId396" xr:uid="{00000000-0004-0000-0000-00008B010000}"/>
-    <hyperlink ref="C430" r:id="rId397" xr:uid="{00000000-0004-0000-0000-00008C010000}"/>
-    <hyperlink ref="C431" r:id="rId398" xr:uid="{00000000-0004-0000-0000-00008D010000}"/>
-    <hyperlink ref="C432" r:id="rId399" xr:uid="{00000000-0004-0000-0000-00008E010000}"/>
-    <hyperlink ref="C433" r:id="rId400" xr:uid="{00000000-0004-0000-0000-00008F010000}"/>
-    <hyperlink ref="C434" r:id="rId401" xr:uid="{00000000-0004-0000-0000-000090010000}"/>
-    <hyperlink ref="C435" r:id="rId402" xr:uid="{00000000-0004-0000-0000-000091010000}"/>
-    <hyperlink ref="C436" r:id="rId403" xr:uid="{00000000-0004-0000-0000-000092010000}"/>
-    <hyperlink ref="C437" r:id="rId404" xr:uid="{00000000-0004-0000-0000-000093010000}"/>
-    <hyperlink ref="C438" r:id="rId405" xr:uid="{00000000-0004-0000-0000-000094010000}"/>
-    <hyperlink ref="C439" r:id="rId406" xr:uid="{00000000-0004-0000-0000-000095010000}"/>
-    <hyperlink ref="C440" r:id="rId407" xr:uid="{00000000-0004-0000-0000-000096010000}"/>
-    <hyperlink ref="C441" r:id="rId408" xr:uid="{00000000-0004-0000-0000-000097010000}"/>
-    <hyperlink ref="C442" r:id="rId409" xr:uid="{00000000-0004-0000-0000-000098010000}"/>
-    <hyperlink ref="C443" r:id="rId410" xr:uid="{00000000-0004-0000-0000-000099010000}"/>
-    <hyperlink ref="C444" r:id="rId411" xr:uid="{00000000-0004-0000-0000-00009A010000}"/>
-    <hyperlink ref="C445" r:id="rId412" xr:uid="{00000000-0004-0000-0000-00009B010000}"/>
-    <hyperlink ref="C446" r:id="rId413" xr:uid="{00000000-0004-0000-0000-00009C010000}"/>
-    <hyperlink ref="C447" r:id="rId414" xr:uid="{00000000-0004-0000-0000-00009D010000}"/>
-    <hyperlink ref="C448" r:id="rId415" xr:uid="{00000000-0004-0000-0000-00009E010000}"/>
-    <hyperlink ref="C449" r:id="rId416" xr:uid="{00000000-0004-0000-0000-00009F010000}"/>
-    <hyperlink ref="C450" r:id="rId417" xr:uid="{00000000-0004-0000-0000-0000A0010000}"/>
-    <hyperlink ref="C451" r:id="rId418" xr:uid="{00000000-0004-0000-0000-0000A1010000}"/>
-    <hyperlink ref="C452" r:id="rId419" xr:uid="{00000000-0004-0000-0000-0000A2010000}"/>
-    <hyperlink ref="C453" r:id="rId420" xr:uid="{00000000-0004-0000-0000-0000A3010000}"/>
-    <hyperlink ref="C454" r:id="rId421" xr:uid="{00000000-0004-0000-0000-0000A4010000}"/>
-    <hyperlink ref="C455" r:id="rId422" xr:uid="{00000000-0004-0000-0000-0000A5010000}"/>
-    <hyperlink ref="C456" r:id="rId423" xr:uid="{00000000-0004-0000-0000-0000A6010000}"/>
-    <hyperlink ref="C457" r:id="rId424" xr:uid="{00000000-0004-0000-0000-0000A7010000}"/>
-    <hyperlink ref="C458" r:id="rId425" xr:uid="{00000000-0004-0000-0000-0000A8010000}"/>
-    <hyperlink ref="C459" r:id="rId426" xr:uid="{00000000-0004-0000-0000-0000A9010000}"/>
-    <hyperlink ref="C460" r:id="rId427" xr:uid="{00000000-0004-0000-0000-0000AA010000}"/>
-    <hyperlink ref="C461" r:id="rId428" xr:uid="{00000000-0004-0000-0000-0000AB010000}"/>
-    <hyperlink ref="C462" r:id="rId429" xr:uid="{00000000-0004-0000-0000-0000AC010000}"/>
-    <hyperlink ref="C463" r:id="rId430" xr:uid="{00000000-0004-0000-0000-0000AD010000}"/>
-    <hyperlink ref="C464" r:id="rId431" xr:uid="{00000000-0004-0000-0000-0000AE010000}"/>
-    <hyperlink ref="C465" r:id="rId432" xr:uid="{00000000-0004-0000-0000-0000AF010000}"/>
-    <hyperlink ref="C466" r:id="rId433" xr:uid="{00000000-0004-0000-0000-0000B0010000}"/>
-    <hyperlink ref="C467" r:id="rId434" xr:uid="{00000000-0004-0000-0000-0000B1010000}"/>
-    <hyperlink ref="C468" r:id="rId435" xr:uid="{00000000-0004-0000-0000-0000B2010000}"/>
-    <hyperlink ref="C469" r:id="rId436" xr:uid="{00000000-0004-0000-0000-0000B3010000}"/>
-    <hyperlink ref="C472" r:id="rId437" xr:uid="{00000000-0004-0000-0000-0000B4010000}"/>
-    <hyperlink ref="C473" r:id="rId438" xr:uid="{00000000-0004-0000-0000-0000B5010000}"/>
-    <hyperlink ref="C474" r:id="rId439" xr:uid="{00000000-0004-0000-0000-0000B6010000}"/>
-    <hyperlink ref="C475" r:id="rId440" xr:uid="{00000000-0004-0000-0000-0000B7010000}"/>
-    <hyperlink ref="C476" r:id="rId441" xr:uid="{00000000-0004-0000-0000-0000B8010000}"/>
-    <hyperlink ref="C477" r:id="rId442" xr:uid="{00000000-0004-0000-0000-0000B9010000}"/>
-    <hyperlink ref="C478" r:id="rId443" xr:uid="{00000000-0004-0000-0000-0000BA010000}"/>
-    <hyperlink ref="C479" r:id="rId444" xr:uid="{00000000-0004-0000-0000-0000BB010000}"/>
-    <hyperlink ref="C480" r:id="rId445" location=":~:text=Given%20an%20integer%20n%2C%20calculate,*%2C%20%2F%20and%20pow().&amp;text=A%20Simple%20Solution%20is%20to%20repeatedly%20add%20n%20to%20result." xr:uid="{00000000-0004-0000-0000-0000BC010000}"/>
-    <hyperlink ref="C481" r:id="rId446" xr:uid="{00000000-0004-0000-0000-0000BD010000}"/>
+    <hyperlink ref="C141" r:id="rId127" xr:uid="{00000000-0004-0000-0000-00007F000000}"/>
+    <hyperlink ref="C142" r:id="rId128" xr:uid="{00000000-0004-0000-0000-000080000000}"/>
+    <hyperlink ref="C143" r:id="rId129" xr:uid="{00000000-0004-0000-0000-000081000000}"/>
+    <hyperlink ref="C144" r:id="rId130" xr:uid="{00000000-0004-0000-0000-000082000000}"/>
+    <hyperlink ref="C145" r:id="rId131" xr:uid="{00000000-0004-0000-0000-000083000000}"/>
+    <hyperlink ref="C146" r:id="rId132" xr:uid="{00000000-0004-0000-0000-000084000000}"/>
+    <hyperlink ref="C147" r:id="rId133" xr:uid="{00000000-0004-0000-0000-000085000000}"/>
+    <hyperlink ref="C148" r:id="rId134" xr:uid="{00000000-0004-0000-0000-000086000000}"/>
+    <hyperlink ref="C149" r:id="rId135" xr:uid="{00000000-0004-0000-0000-000087000000}"/>
+    <hyperlink ref="C150" r:id="rId136" xr:uid="{00000000-0004-0000-0000-000088000000}"/>
+    <hyperlink ref="C151" r:id="rId137" xr:uid="{00000000-0004-0000-0000-000089000000}"/>
+    <hyperlink ref="C152" r:id="rId138" xr:uid="{00000000-0004-0000-0000-00008A000000}"/>
+    <hyperlink ref="C153" r:id="rId139" xr:uid="{00000000-0004-0000-0000-00008B000000}"/>
+    <hyperlink ref="C154" r:id="rId140" xr:uid="{00000000-0004-0000-0000-00008C000000}"/>
+    <hyperlink ref="C155" r:id="rId141" xr:uid="{00000000-0004-0000-0000-00008D000000}"/>
+    <hyperlink ref="C156" r:id="rId142" xr:uid="{00000000-0004-0000-0000-00008E000000}"/>
+    <hyperlink ref="C157" r:id="rId143" xr:uid="{00000000-0004-0000-0000-00008F000000}"/>
+    <hyperlink ref="C158" r:id="rId144" xr:uid="{00000000-0004-0000-0000-000090000000}"/>
+    <hyperlink ref="C159" r:id="rId145" xr:uid="{00000000-0004-0000-0000-000091000000}"/>
+    <hyperlink ref="C160" r:id="rId146" xr:uid="{00000000-0004-0000-0000-000092000000}"/>
+    <hyperlink ref="C161" r:id="rId147" xr:uid="{00000000-0004-0000-0000-000093000000}"/>
+    <hyperlink ref="C162" r:id="rId148" xr:uid="{00000000-0004-0000-0000-000094000000}"/>
+    <hyperlink ref="C163" r:id="rId149" xr:uid="{00000000-0004-0000-0000-000095000000}"/>
+    <hyperlink ref="C166" r:id="rId150" xr:uid="{00000000-0004-0000-0000-000096000000}"/>
+    <hyperlink ref="C167" r:id="rId151" xr:uid="{00000000-0004-0000-0000-000097000000}"/>
+    <hyperlink ref="C168" r:id="rId152" xr:uid="{00000000-0004-0000-0000-000098000000}"/>
+    <hyperlink ref="C169" r:id="rId153" xr:uid="{00000000-0004-0000-0000-000099000000}"/>
+    <hyperlink ref="C170" r:id="rId154" xr:uid="{00000000-0004-0000-0000-00009A000000}"/>
+    <hyperlink ref="C171" r:id="rId155" xr:uid="{00000000-0004-0000-0000-00009B000000}"/>
+    <hyperlink ref="C172" r:id="rId156" xr:uid="{00000000-0004-0000-0000-00009C000000}"/>
+    <hyperlink ref="C173" r:id="rId157" xr:uid="{00000000-0004-0000-0000-00009D000000}"/>
+    <hyperlink ref="C174" r:id="rId158" xr:uid="{00000000-0004-0000-0000-00009E000000}"/>
+    <hyperlink ref="C177" r:id="rId159" xr:uid="{00000000-0004-0000-0000-00009F000000}"/>
+    <hyperlink ref="C178" r:id="rId160" xr:uid="{00000000-0004-0000-0000-0000A0000000}"/>
+    <hyperlink ref="C179" r:id="rId161" xr:uid="{00000000-0004-0000-0000-0000A1000000}"/>
+    <hyperlink ref="C180" r:id="rId162" xr:uid="{00000000-0004-0000-0000-0000A2000000}"/>
+    <hyperlink ref="C181" r:id="rId163" xr:uid="{00000000-0004-0000-0000-0000A3000000}"/>
+    <hyperlink ref="C182" r:id="rId164" xr:uid="{00000000-0004-0000-0000-0000A4000000}"/>
+    <hyperlink ref="C183" r:id="rId165" xr:uid="{00000000-0004-0000-0000-0000A5000000}"/>
+    <hyperlink ref="C184" r:id="rId166" xr:uid="{00000000-0004-0000-0000-0000A6000000}"/>
+    <hyperlink ref="C185" r:id="rId167" xr:uid="{00000000-0004-0000-0000-0000A7000000}"/>
+    <hyperlink ref="C186" r:id="rId168" xr:uid="{00000000-0004-0000-0000-0000A8000000}"/>
+    <hyperlink ref="C187" r:id="rId169" xr:uid="{00000000-0004-0000-0000-0000A9000000}"/>
+    <hyperlink ref="C188" r:id="rId170" xr:uid="{00000000-0004-0000-0000-0000AA000000}"/>
+    <hyperlink ref="C189" r:id="rId171" xr:uid="{00000000-0004-0000-0000-0000AB000000}"/>
+    <hyperlink ref="C190" r:id="rId172" xr:uid="{00000000-0004-0000-0000-0000AC000000}"/>
+    <hyperlink ref="C191" r:id="rId173" xr:uid="{00000000-0004-0000-0000-0000AD000000}"/>
+    <hyperlink ref="C192" r:id="rId174" xr:uid="{00000000-0004-0000-0000-0000AE000000}"/>
+    <hyperlink ref="C193" r:id="rId175" xr:uid="{00000000-0004-0000-0000-0000AF000000}"/>
+    <hyperlink ref="C194" r:id="rId176" xr:uid="{00000000-0004-0000-0000-0000B0000000}"/>
+    <hyperlink ref="C195" r:id="rId177" xr:uid="{00000000-0004-0000-0000-0000B1000000}"/>
+    <hyperlink ref="C196" r:id="rId178" xr:uid="{00000000-0004-0000-0000-0000B2000000}"/>
+    <hyperlink ref="C197" r:id="rId179" location=":~:text=Given%20the%20array%20representation%20of,it%20into%20Binary%20Search%20Tree.&amp;text=Swap%201%3A%20Swap%20node%208,node%209%20with%20node%2010." xr:uid="{00000000-0004-0000-0000-0000B3000000}"/>
+    <hyperlink ref="C198" r:id="rId180" xr:uid="{00000000-0004-0000-0000-0000B4000000}"/>
+    <hyperlink ref="C199" r:id="rId181" xr:uid="{00000000-0004-0000-0000-0000B5000000}"/>
+    <hyperlink ref="C200" r:id="rId182" xr:uid="{00000000-0004-0000-0000-0000B6000000}"/>
+    <hyperlink ref="C201" r:id="rId183" xr:uid="{00000000-0004-0000-0000-0000B7000000}"/>
+    <hyperlink ref="C202" r:id="rId184" xr:uid="{00000000-0004-0000-0000-0000B8000000}"/>
+    <hyperlink ref="C203" r:id="rId185" location=":~:text=Since%20the%20graph%20is%20undirected,graph%20is%20connected%2C%20otherwise%20not." xr:uid="{00000000-0004-0000-0000-0000B9000000}"/>
+    <hyperlink ref="C204" r:id="rId186" xr:uid="{00000000-0004-0000-0000-0000BA000000}"/>
+    <hyperlink ref="C205" r:id="rId187" xr:uid="{00000000-0004-0000-0000-0000BB000000}"/>
+    <hyperlink ref="C206" r:id="rId188" xr:uid="{00000000-0004-0000-0000-0000BC000000}"/>
+    <hyperlink ref="C207" r:id="rId189" xr:uid="{00000000-0004-0000-0000-0000BD000000}"/>
+    <hyperlink ref="C208" r:id="rId190" xr:uid="{00000000-0004-0000-0000-0000BE000000}"/>
+    <hyperlink ref="C209" r:id="rId191" xr:uid="{00000000-0004-0000-0000-0000BF000000}"/>
+    <hyperlink ref="C210" r:id="rId192" xr:uid="{00000000-0004-0000-0000-0000C0000000}"/>
+    <hyperlink ref="C211" r:id="rId193" xr:uid="{00000000-0004-0000-0000-0000C1000000}"/>
+    <hyperlink ref="C214" r:id="rId194" xr:uid="{00000000-0004-0000-0000-0000C2000000}"/>
+    <hyperlink ref="C215" r:id="rId195" xr:uid="{00000000-0004-0000-0000-0000C3000000}"/>
+    <hyperlink ref="C216" r:id="rId196" xr:uid="{00000000-0004-0000-0000-0000C4000000}"/>
+    <hyperlink ref="C217" r:id="rId197" xr:uid="{00000000-0004-0000-0000-0000C5000000}"/>
+    <hyperlink ref="C218" r:id="rId198" xr:uid="{00000000-0004-0000-0000-0000C6000000}"/>
+    <hyperlink ref="C219" r:id="rId199" xr:uid="{00000000-0004-0000-0000-0000C7000000}"/>
+    <hyperlink ref="C220" r:id="rId200" xr:uid="{00000000-0004-0000-0000-0000C8000000}"/>
+    <hyperlink ref="C221" r:id="rId201" xr:uid="{00000000-0004-0000-0000-0000C9000000}"/>
+    <hyperlink ref="C222" r:id="rId202" xr:uid="{00000000-0004-0000-0000-0000CA000000}"/>
+    <hyperlink ref="C223" r:id="rId203" xr:uid="{00000000-0004-0000-0000-0000CB000000}"/>
+    <hyperlink ref="C224" r:id="rId204" xr:uid="{00000000-0004-0000-0000-0000CC000000}"/>
+    <hyperlink ref="C225" r:id="rId205" xr:uid="{00000000-0004-0000-0000-0000CD000000}"/>
+    <hyperlink ref="C226" r:id="rId206" xr:uid="{00000000-0004-0000-0000-0000CE000000}"/>
+    <hyperlink ref="C227" r:id="rId207" xr:uid="{00000000-0004-0000-0000-0000CF000000}"/>
+    <hyperlink ref="C228" r:id="rId208" xr:uid="{00000000-0004-0000-0000-0000D0000000}"/>
+    <hyperlink ref="C229" r:id="rId209" xr:uid="{00000000-0004-0000-0000-0000D1000000}"/>
+    <hyperlink ref="C230" r:id="rId210" xr:uid="{00000000-0004-0000-0000-0000D2000000}"/>
+    <hyperlink ref="C231" r:id="rId211" xr:uid="{00000000-0004-0000-0000-0000D3000000}"/>
+    <hyperlink ref="C232" r:id="rId212" xr:uid="{00000000-0004-0000-0000-0000D4000000}"/>
+    <hyperlink ref="C233" r:id="rId213" xr:uid="{00000000-0004-0000-0000-0000D5000000}"/>
+    <hyperlink ref="C234" r:id="rId214" xr:uid="{00000000-0004-0000-0000-0000D6000000}"/>
+    <hyperlink ref="C235" r:id="rId215" xr:uid="{00000000-0004-0000-0000-0000D7000000}"/>
+    <hyperlink ref="C238" r:id="rId216" xr:uid="{00000000-0004-0000-0000-0000D8000000}"/>
+    <hyperlink ref="C239" r:id="rId217" xr:uid="{00000000-0004-0000-0000-0000D9000000}"/>
+    <hyperlink ref="C240" r:id="rId218" xr:uid="{00000000-0004-0000-0000-0000DA000000}"/>
+    <hyperlink ref="C241" r:id="rId219" xr:uid="{00000000-0004-0000-0000-0000DB000000}"/>
+    <hyperlink ref="C242" r:id="rId220" xr:uid="{00000000-0004-0000-0000-0000DC000000}"/>
+    <hyperlink ref="C243" r:id="rId221" xr:uid="{00000000-0004-0000-0000-0000DD000000}"/>
+    <hyperlink ref="C244" r:id="rId222" xr:uid="{00000000-0004-0000-0000-0000DE000000}"/>
+    <hyperlink ref="C245" r:id="rId223" xr:uid="{00000000-0004-0000-0000-0000DF000000}"/>
+    <hyperlink ref="C246" r:id="rId224" xr:uid="{00000000-0004-0000-0000-0000E0000000}"/>
+    <hyperlink ref="C247" r:id="rId225" xr:uid="{00000000-0004-0000-0000-0000E1000000}"/>
+    <hyperlink ref="C248" r:id="rId226" xr:uid="{00000000-0004-0000-0000-0000E2000000}"/>
+    <hyperlink ref="C249" r:id="rId227" xr:uid="{00000000-0004-0000-0000-0000E3000000}"/>
+    <hyperlink ref="C250" r:id="rId228" xr:uid="{00000000-0004-0000-0000-0000E4000000}"/>
+    <hyperlink ref="C251" r:id="rId229" xr:uid="{00000000-0004-0000-0000-0000E5000000}"/>
+    <hyperlink ref="C252" r:id="rId230" xr:uid="{00000000-0004-0000-0000-0000E6000000}"/>
+    <hyperlink ref="C253" r:id="rId231" xr:uid="{00000000-0004-0000-0000-0000E7000000}"/>
+    <hyperlink ref="C254" r:id="rId232" xr:uid="{00000000-0004-0000-0000-0000E8000000}"/>
+    <hyperlink ref="C255" r:id="rId233" xr:uid="{00000000-0004-0000-0000-0000E9000000}"/>
+    <hyperlink ref="C256" r:id="rId234" xr:uid="{00000000-0004-0000-0000-0000EA000000}"/>
+    <hyperlink ref="C257" r:id="rId235" location=":~:text=It%20consists%20of%20two%20steps,result%20to%20the%20sum%20S." xr:uid="{00000000-0004-0000-0000-0000EB000000}"/>
+    <hyperlink ref="C258" r:id="rId236" xr:uid="{00000000-0004-0000-0000-0000EC000000}"/>
+    <hyperlink ref="C259" r:id="rId237" xr:uid="{00000000-0004-0000-0000-0000ED000000}"/>
+    <hyperlink ref="C260" r:id="rId238" xr:uid="{00000000-0004-0000-0000-0000EE000000}"/>
+    <hyperlink ref="C261" r:id="rId239" xr:uid="{00000000-0004-0000-0000-0000EF000000}"/>
+    <hyperlink ref="C262" r:id="rId240" xr:uid="{00000000-0004-0000-0000-0000F0000000}"/>
+    <hyperlink ref="C263" r:id="rId241" xr:uid="{00000000-0004-0000-0000-0000F1000000}"/>
+    <hyperlink ref="C264" r:id="rId242" xr:uid="{00000000-0004-0000-0000-0000F2000000}"/>
+    <hyperlink ref="C265" r:id="rId243" xr:uid="{00000000-0004-0000-0000-0000F3000000}"/>
+    <hyperlink ref="C266" r:id="rId244" xr:uid="{00000000-0004-0000-0000-0000F4000000}"/>
+    <hyperlink ref="C267" r:id="rId245" xr:uid="{00000000-0004-0000-0000-0000F5000000}"/>
+    <hyperlink ref="C268" r:id="rId246" xr:uid="{00000000-0004-0000-0000-0000F6000000}"/>
+    <hyperlink ref="C269" r:id="rId247" xr:uid="{00000000-0004-0000-0000-0000F7000000}"/>
+    <hyperlink ref="C270" r:id="rId248" xr:uid="{00000000-0004-0000-0000-0000F8000000}"/>
+    <hyperlink ref="C271" r:id="rId249" xr:uid="{00000000-0004-0000-0000-0000F9000000}"/>
+    <hyperlink ref="C272" r:id="rId250" xr:uid="{00000000-0004-0000-0000-0000FA000000}"/>
+    <hyperlink ref="C275" r:id="rId251" xr:uid="{00000000-0004-0000-0000-0000FB000000}"/>
+    <hyperlink ref="C276" r:id="rId252" xr:uid="{00000000-0004-0000-0000-0000FC000000}"/>
+    <hyperlink ref="C277" r:id="rId253" xr:uid="{00000000-0004-0000-0000-0000FD000000}"/>
+    <hyperlink ref="C278" r:id="rId254" xr:uid="{00000000-0004-0000-0000-0000FE000000}"/>
+    <hyperlink ref="C279" r:id="rId255" xr:uid="{00000000-0004-0000-0000-0000FF000000}"/>
+    <hyperlink ref="C280" r:id="rId256" xr:uid="{00000000-0004-0000-0000-000000010000}"/>
+    <hyperlink ref="C281" r:id="rId257" xr:uid="{00000000-0004-0000-0000-000001010000}"/>
+    <hyperlink ref="C282" r:id="rId258" xr:uid="{00000000-0004-0000-0000-000002010000}"/>
+    <hyperlink ref="C283" r:id="rId259" xr:uid="{00000000-0004-0000-0000-000003010000}"/>
+    <hyperlink ref="C284" r:id="rId260" xr:uid="{00000000-0004-0000-0000-000004010000}"/>
+    <hyperlink ref="C285" r:id="rId261" xr:uid="{00000000-0004-0000-0000-000005010000}"/>
+    <hyperlink ref="C286" r:id="rId262" xr:uid="{00000000-0004-0000-0000-000006010000}"/>
+    <hyperlink ref="C287" r:id="rId263" xr:uid="{00000000-0004-0000-0000-000007010000}"/>
+    <hyperlink ref="C288" r:id="rId264" xr:uid="{00000000-0004-0000-0000-000008010000}"/>
+    <hyperlink ref="C289" r:id="rId265" xr:uid="{00000000-0004-0000-0000-000009010000}"/>
+    <hyperlink ref="C290" r:id="rId266" xr:uid="{00000000-0004-0000-0000-00000A010000}"/>
+    <hyperlink ref="C291" r:id="rId267" xr:uid="{00000000-0004-0000-0000-00000B010000}"/>
+    <hyperlink ref="C292" r:id="rId268" xr:uid="{00000000-0004-0000-0000-00000C010000}"/>
+    <hyperlink ref="C293" r:id="rId269" xr:uid="{00000000-0004-0000-0000-00000D010000}"/>
+    <hyperlink ref="C296" r:id="rId270" xr:uid="{00000000-0004-0000-0000-00000E010000}"/>
+    <hyperlink ref="C297" r:id="rId271" xr:uid="{00000000-0004-0000-0000-00000F010000}"/>
+    <hyperlink ref="C298" r:id="rId272" xr:uid="{00000000-0004-0000-0000-000010010000}"/>
+    <hyperlink ref="C299" r:id="rId273" xr:uid="{00000000-0004-0000-0000-000011010000}"/>
+    <hyperlink ref="C300" r:id="rId274" xr:uid="{00000000-0004-0000-0000-000012010000}"/>
+    <hyperlink ref="C301" r:id="rId275" xr:uid="{00000000-0004-0000-0000-000013010000}"/>
+    <hyperlink ref="C302" r:id="rId276" xr:uid="{00000000-0004-0000-0000-000014010000}"/>
+    <hyperlink ref="C303" r:id="rId277" xr:uid="{00000000-0004-0000-0000-000015010000}"/>
+    <hyperlink ref="C304" r:id="rId278" xr:uid="{00000000-0004-0000-0000-000016010000}"/>
+    <hyperlink ref="C305" r:id="rId279" xr:uid="{00000000-0004-0000-0000-000017010000}"/>
+    <hyperlink ref="C306" r:id="rId280" location=":~:text=The%20stack%20organization%20is%20very,i.e.%2C%20A%20%2B%20B)." xr:uid="{00000000-0004-0000-0000-000018010000}"/>
+    <hyperlink ref="C307" r:id="rId281" xr:uid="{00000000-0004-0000-0000-000019010000}"/>
+    <hyperlink ref="C308" r:id="rId282" xr:uid="{00000000-0004-0000-0000-00001A010000}"/>
+    <hyperlink ref="C309" r:id="rId283" xr:uid="{00000000-0004-0000-0000-00001B010000}"/>
+    <hyperlink ref="C310" r:id="rId284" xr:uid="{00000000-0004-0000-0000-00001C010000}"/>
+    <hyperlink ref="C311" r:id="rId285" xr:uid="{00000000-0004-0000-0000-00001D010000}"/>
+    <hyperlink ref="C312" r:id="rId286" xr:uid="{00000000-0004-0000-0000-00001E010000}"/>
+    <hyperlink ref="C313" r:id="rId287" xr:uid="{00000000-0004-0000-0000-00001F010000}"/>
+    <hyperlink ref="C314" r:id="rId288" xr:uid="{00000000-0004-0000-0000-000020010000}"/>
+    <hyperlink ref="C315" r:id="rId289" xr:uid="{00000000-0004-0000-0000-000021010000}"/>
+    <hyperlink ref="C316" r:id="rId290" xr:uid="{00000000-0004-0000-0000-000022010000}"/>
+    <hyperlink ref="C317" r:id="rId291" xr:uid="{00000000-0004-0000-0000-000023010000}"/>
+    <hyperlink ref="C318" r:id="rId292" xr:uid="{00000000-0004-0000-0000-000024010000}"/>
+    <hyperlink ref="C319" r:id="rId293" xr:uid="{00000000-0004-0000-0000-000025010000}"/>
+    <hyperlink ref="C320" r:id="rId294" xr:uid="{00000000-0004-0000-0000-000026010000}"/>
+    <hyperlink ref="C321" r:id="rId295" xr:uid="{00000000-0004-0000-0000-000027010000}"/>
+    <hyperlink ref="C322" r:id="rId296" xr:uid="{00000000-0004-0000-0000-000028010000}"/>
+    <hyperlink ref="C323" r:id="rId297" xr:uid="{00000000-0004-0000-0000-000029010000}"/>
+    <hyperlink ref="C324" r:id="rId298" xr:uid="{00000000-0004-0000-0000-00002A010000}"/>
+    <hyperlink ref="C325" r:id="rId299" xr:uid="{00000000-0004-0000-0000-00002B010000}"/>
+    <hyperlink ref="C326" r:id="rId300" xr:uid="{00000000-0004-0000-0000-00002C010000}"/>
+    <hyperlink ref="C327" r:id="rId301" xr:uid="{00000000-0004-0000-0000-00002D010000}"/>
+    <hyperlink ref="C328" r:id="rId302" xr:uid="{00000000-0004-0000-0000-00002E010000}"/>
+    <hyperlink ref="C329" r:id="rId303" xr:uid="{00000000-0004-0000-0000-00002F010000}"/>
+    <hyperlink ref="C330" r:id="rId304" xr:uid="{00000000-0004-0000-0000-000030010000}"/>
+    <hyperlink ref="C331" r:id="rId305" xr:uid="{00000000-0004-0000-0000-000031010000}"/>
+    <hyperlink ref="C332" r:id="rId306" xr:uid="{00000000-0004-0000-0000-000032010000}"/>
+    <hyperlink ref="C333" r:id="rId307" xr:uid="{00000000-0004-0000-0000-000033010000}"/>
+    <hyperlink ref="C336" r:id="rId308" xr:uid="{00000000-0004-0000-0000-000034010000}"/>
+    <hyperlink ref="C337" r:id="rId309" xr:uid="{00000000-0004-0000-0000-000035010000}"/>
+    <hyperlink ref="C338" r:id="rId310" xr:uid="{00000000-0004-0000-0000-000036010000}"/>
+    <hyperlink ref="C339" r:id="rId311" xr:uid="{00000000-0004-0000-0000-000037010000}"/>
+    <hyperlink ref="C340" r:id="rId312" xr:uid="{00000000-0004-0000-0000-000038010000}"/>
+    <hyperlink ref="C341" r:id="rId313" xr:uid="{00000000-0004-0000-0000-000039010000}"/>
+    <hyperlink ref="C342" r:id="rId314" xr:uid="{00000000-0004-0000-0000-00003A010000}"/>
+    <hyperlink ref="C343" r:id="rId315" xr:uid="{00000000-0004-0000-0000-00003B010000}"/>
+    <hyperlink ref="C344" r:id="rId316" xr:uid="{00000000-0004-0000-0000-00003C010000}"/>
+    <hyperlink ref="C345" r:id="rId317" xr:uid="{00000000-0004-0000-0000-00003D010000}"/>
+    <hyperlink ref="C346" r:id="rId318" xr:uid="{00000000-0004-0000-0000-00003E010000}"/>
+    <hyperlink ref="C347" r:id="rId319" xr:uid="{00000000-0004-0000-0000-00003F010000}"/>
+    <hyperlink ref="C348" r:id="rId320" xr:uid="{00000000-0004-0000-0000-000040010000}"/>
+    <hyperlink ref="C349" r:id="rId321" xr:uid="{00000000-0004-0000-0000-000041010000}"/>
+    <hyperlink ref="C350" r:id="rId322" xr:uid="{00000000-0004-0000-0000-000042010000}"/>
+    <hyperlink ref="C351" r:id="rId323" xr:uid="{00000000-0004-0000-0000-000043010000}"/>
+    <hyperlink ref="C352" r:id="rId324" xr:uid="{00000000-0004-0000-0000-000044010000}"/>
+    <hyperlink ref="C353" r:id="rId325" xr:uid="{00000000-0004-0000-0000-000045010000}"/>
+    <hyperlink ref="C356" r:id="rId326" xr:uid="{00000000-0004-0000-0000-000046010000}"/>
+    <hyperlink ref="C357" r:id="rId327" xr:uid="{00000000-0004-0000-0000-000047010000}"/>
+    <hyperlink ref="C358" r:id="rId328" xr:uid="{00000000-0004-0000-0000-000048010000}"/>
+    <hyperlink ref="C359" r:id="rId329" xr:uid="{00000000-0004-0000-0000-000049010000}"/>
+    <hyperlink ref="C360" r:id="rId330" xr:uid="{00000000-0004-0000-0000-00004A010000}"/>
+    <hyperlink ref="C361" r:id="rId331" xr:uid="{00000000-0004-0000-0000-00004B010000}"/>
+    <hyperlink ref="C362" r:id="rId332" xr:uid="{00000000-0004-0000-0000-00004C010000}"/>
+    <hyperlink ref="C363" r:id="rId333" xr:uid="{00000000-0004-0000-0000-00004D010000}"/>
+    <hyperlink ref="C364" r:id="rId334" xr:uid="{00000000-0004-0000-0000-00004E010000}"/>
+    <hyperlink ref="C365" r:id="rId335" xr:uid="{00000000-0004-0000-0000-00004F010000}"/>
+    <hyperlink ref="C366" r:id="rId336" xr:uid="{00000000-0004-0000-0000-000050010000}"/>
+    <hyperlink ref="C367" r:id="rId337" xr:uid="{00000000-0004-0000-0000-000051010000}"/>
+    <hyperlink ref="C368" r:id="rId338" xr:uid="{00000000-0004-0000-0000-000052010000}"/>
+    <hyperlink ref="C369" r:id="rId339" xr:uid="{00000000-0004-0000-0000-000053010000}"/>
+    <hyperlink ref="C370" r:id="rId340" xr:uid="{00000000-0004-0000-0000-000054010000}"/>
+    <hyperlink ref="C371" r:id="rId341" xr:uid="{00000000-0004-0000-0000-000055010000}"/>
+    <hyperlink ref="C372" r:id="rId342" xr:uid="{00000000-0004-0000-0000-000056010000}"/>
+    <hyperlink ref="C373" r:id="rId343" xr:uid="{00000000-0004-0000-0000-000057010000}"/>
+    <hyperlink ref="C374" r:id="rId344" xr:uid="{00000000-0004-0000-0000-000058010000}"/>
+    <hyperlink ref="C375" r:id="rId345" xr:uid="{00000000-0004-0000-0000-000059010000}"/>
+    <hyperlink ref="C376" r:id="rId346" xr:uid="{00000000-0004-0000-0000-00005A010000}"/>
+    <hyperlink ref="C377" r:id="rId347" xr:uid="{00000000-0004-0000-0000-00005B010000}"/>
+    <hyperlink ref="C378" r:id="rId348" xr:uid="{00000000-0004-0000-0000-00005C010000}"/>
+    <hyperlink ref="C379" r:id="rId349" location=":~:text=Graph%20coloring%20problem%20is%20to,are%20colored%20using%20same%20color." xr:uid="{00000000-0004-0000-0000-00005D010000}"/>
+    <hyperlink ref="C380" r:id="rId350" xr:uid="{00000000-0004-0000-0000-00005E010000}"/>
+    <hyperlink ref="C381" r:id="rId351" xr:uid="{00000000-0004-0000-0000-00005F010000}"/>
+    <hyperlink ref="C382" r:id="rId352" xr:uid="{00000000-0004-0000-0000-000060010000}"/>
+    <hyperlink ref="C383" r:id="rId353" xr:uid="{00000000-0004-0000-0000-000061010000}"/>
+    <hyperlink ref="C384" r:id="rId354" xr:uid="{00000000-0004-0000-0000-000062010000}"/>
+    <hyperlink ref="C385" r:id="rId355" xr:uid="{00000000-0004-0000-0000-000063010000}"/>
+    <hyperlink ref="C386" r:id="rId356" xr:uid="{00000000-0004-0000-0000-000064010000}"/>
+    <hyperlink ref="C387" r:id="rId357" xr:uid="{00000000-0004-0000-0000-000065010000}"/>
+    <hyperlink ref="C388" r:id="rId358" xr:uid="{00000000-0004-0000-0000-000066010000}"/>
+    <hyperlink ref="C389" r:id="rId359" xr:uid="{00000000-0004-0000-0000-000067010000}"/>
+    <hyperlink ref="C390" r:id="rId360" xr:uid="{00000000-0004-0000-0000-000068010000}"/>
+    <hyperlink ref="C391" r:id="rId361" xr:uid="{00000000-0004-0000-0000-000069010000}"/>
+    <hyperlink ref="C392" r:id="rId362" xr:uid="{00000000-0004-0000-0000-00006A010000}"/>
+    <hyperlink ref="C393" r:id="rId363" xr:uid="{00000000-0004-0000-0000-00006B010000}"/>
+    <hyperlink ref="C394" r:id="rId364" xr:uid="{00000000-0004-0000-0000-00006C010000}"/>
+    <hyperlink ref="C395" r:id="rId365" xr:uid="{00000000-0004-0000-0000-00006D010000}"/>
+    <hyperlink ref="C396" r:id="rId366" xr:uid="{00000000-0004-0000-0000-00006E010000}"/>
+    <hyperlink ref="C397" r:id="rId367" xr:uid="{00000000-0004-0000-0000-00006F010000}"/>
+    <hyperlink ref="C398" r:id="rId368" xr:uid="{00000000-0004-0000-0000-000070010000}"/>
+    <hyperlink ref="C399" r:id="rId369" xr:uid="{00000000-0004-0000-0000-000071010000}"/>
+    <hyperlink ref="C402" r:id="rId370" xr:uid="{00000000-0004-0000-0000-000072010000}"/>
+    <hyperlink ref="C403" r:id="rId371" xr:uid="{00000000-0004-0000-0000-000073010000}"/>
+    <hyperlink ref="C404" r:id="rId372" xr:uid="{00000000-0004-0000-0000-000074010000}"/>
+    <hyperlink ref="C405" r:id="rId373" xr:uid="{00000000-0004-0000-0000-000075010000}"/>
+    <hyperlink ref="C406" r:id="rId374" xr:uid="{00000000-0004-0000-0000-000076010000}"/>
+    <hyperlink ref="C407" r:id="rId375" xr:uid="{00000000-0004-0000-0000-000077010000}"/>
+    <hyperlink ref="C410" r:id="rId376" xr:uid="{00000000-0004-0000-0000-000078010000}"/>
+    <hyperlink ref="C411" r:id="rId377" xr:uid="{00000000-0004-0000-0000-000079010000}"/>
+    <hyperlink ref="C412" r:id="rId378" xr:uid="{00000000-0004-0000-0000-00007A010000}"/>
+    <hyperlink ref="C413" r:id="rId379" xr:uid="{00000000-0004-0000-0000-00007B010000}"/>
+    <hyperlink ref="C414" r:id="rId380" xr:uid="{00000000-0004-0000-0000-00007C010000}"/>
+    <hyperlink ref="C415" r:id="rId381" xr:uid="{00000000-0004-0000-0000-00007D010000}"/>
+    <hyperlink ref="C416" r:id="rId382" xr:uid="{00000000-0004-0000-0000-00007E010000}"/>
+    <hyperlink ref="C417" r:id="rId383" xr:uid="{00000000-0004-0000-0000-00007F010000}"/>
+    <hyperlink ref="C418" r:id="rId384" xr:uid="{00000000-0004-0000-0000-000080010000}"/>
+    <hyperlink ref="C419" r:id="rId385" xr:uid="{00000000-0004-0000-0000-000081010000}"/>
+    <hyperlink ref="C420" r:id="rId386" xr:uid="{00000000-0004-0000-0000-000082010000}"/>
+    <hyperlink ref="C421" r:id="rId387" xr:uid="{00000000-0004-0000-0000-000083010000}"/>
+    <hyperlink ref="C422" r:id="rId388" xr:uid="{00000000-0004-0000-0000-000084010000}"/>
+    <hyperlink ref="C423" r:id="rId389" xr:uid="{00000000-0004-0000-0000-000085010000}"/>
+    <hyperlink ref="C424" r:id="rId390" xr:uid="{00000000-0004-0000-0000-000086010000}"/>
+    <hyperlink ref="C425" r:id="rId391" xr:uid="{00000000-0004-0000-0000-000087010000}"/>
+    <hyperlink ref="C426" r:id="rId392" xr:uid="{00000000-0004-0000-0000-000088010000}"/>
+    <hyperlink ref="C427" r:id="rId393" xr:uid="{00000000-0004-0000-0000-000089010000}"/>
+    <hyperlink ref="C428" r:id="rId394" xr:uid="{00000000-0004-0000-0000-00008A010000}"/>
+    <hyperlink ref="C429" r:id="rId395" xr:uid="{00000000-0004-0000-0000-00008B010000}"/>
+    <hyperlink ref="C430" r:id="rId396" xr:uid="{00000000-0004-0000-0000-00008C010000}"/>
+    <hyperlink ref="C431" r:id="rId397" xr:uid="{00000000-0004-0000-0000-00008D010000}"/>
+    <hyperlink ref="C432" r:id="rId398" xr:uid="{00000000-0004-0000-0000-00008E010000}"/>
+    <hyperlink ref="C433" r:id="rId399" xr:uid="{00000000-0004-0000-0000-00008F010000}"/>
+    <hyperlink ref="C434" r:id="rId400" xr:uid="{00000000-0004-0000-0000-000090010000}"/>
+    <hyperlink ref="C435" r:id="rId401" xr:uid="{00000000-0004-0000-0000-000091010000}"/>
+    <hyperlink ref="C436" r:id="rId402" xr:uid="{00000000-0004-0000-0000-000092010000}"/>
+    <hyperlink ref="C437" r:id="rId403" xr:uid="{00000000-0004-0000-0000-000093010000}"/>
+    <hyperlink ref="C438" r:id="rId404" xr:uid="{00000000-0004-0000-0000-000094010000}"/>
+    <hyperlink ref="C439" r:id="rId405" xr:uid="{00000000-0004-0000-0000-000095010000}"/>
+    <hyperlink ref="C440" r:id="rId406" xr:uid="{00000000-0004-0000-0000-000096010000}"/>
+    <hyperlink ref="C441" r:id="rId407" xr:uid="{00000000-0004-0000-0000-000097010000}"/>
+    <hyperlink ref="C442" r:id="rId408" xr:uid="{00000000-0004-0000-0000-000098010000}"/>
+    <hyperlink ref="C443" r:id="rId409" xr:uid="{00000000-0004-0000-0000-000099010000}"/>
+    <hyperlink ref="C444" r:id="rId410" xr:uid="{00000000-0004-0000-0000-00009A010000}"/>
+    <hyperlink ref="C445" r:id="rId411" xr:uid="{00000000-0004-0000-0000-00009B010000}"/>
+    <hyperlink ref="C446" r:id="rId412" xr:uid="{00000000-0004-0000-0000-00009C010000}"/>
+    <hyperlink ref="C447" r:id="rId413" xr:uid="{00000000-0004-0000-0000-00009D010000}"/>
+    <hyperlink ref="C448" r:id="rId414" xr:uid="{00000000-0004-0000-0000-00009E010000}"/>
+    <hyperlink ref="C449" r:id="rId415" xr:uid="{00000000-0004-0000-0000-00009F010000}"/>
+    <hyperlink ref="C450" r:id="rId416" xr:uid="{00000000-0004-0000-0000-0000A0010000}"/>
+    <hyperlink ref="C451" r:id="rId417" xr:uid="{00000000-0004-0000-0000-0000A1010000}"/>
+    <hyperlink ref="C452" r:id="rId418" xr:uid="{00000000-0004-0000-0000-0000A2010000}"/>
+    <hyperlink ref="C453" r:id="rId419" xr:uid="{00000000-0004-0000-0000-0000A3010000}"/>
+    <hyperlink ref="C454" r:id="rId420" xr:uid="{00000000-0004-0000-0000-0000A4010000}"/>
+    <hyperlink ref="C455" r:id="rId421" xr:uid="{00000000-0004-0000-0000-0000A5010000}"/>
+    <hyperlink ref="C456" r:id="rId422" xr:uid="{00000000-0004-0000-0000-0000A6010000}"/>
+    <hyperlink ref="C457" r:id="rId423" xr:uid="{00000000-0004-0000-0000-0000A7010000}"/>
+    <hyperlink ref="C458" r:id="rId424" xr:uid="{00000000-0004-0000-0000-0000A8010000}"/>
+    <hyperlink ref="C459" r:id="rId425" xr:uid="{00000000-0004-0000-0000-0000A9010000}"/>
+    <hyperlink ref="C460" r:id="rId426" xr:uid="{00000000-0004-0000-0000-0000AA010000}"/>
+    <hyperlink ref="C461" r:id="rId427" xr:uid="{00000000-0004-0000-0000-0000AB010000}"/>
+    <hyperlink ref="C462" r:id="rId428" xr:uid="{00000000-0004-0000-0000-0000AC010000}"/>
+    <hyperlink ref="C463" r:id="rId429" xr:uid="{00000000-0004-0000-0000-0000AD010000}"/>
+    <hyperlink ref="C464" r:id="rId430" xr:uid="{00000000-0004-0000-0000-0000AE010000}"/>
+    <hyperlink ref="C465" r:id="rId431" xr:uid="{00000000-0004-0000-0000-0000AF010000}"/>
+    <hyperlink ref="C466" r:id="rId432" xr:uid="{00000000-0004-0000-0000-0000B0010000}"/>
+    <hyperlink ref="C467" r:id="rId433" xr:uid="{00000000-0004-0000-0000-0000B1010000}"/>
+    <hyperlink ref="C468" r:id="rId434" xr:uid="{00000000-0004-0000-0000-0000B2010000}"/>
+    <hyperlink ref="C469" r:id="rId435" xr:uid="{00000000-0004-0000-0000-0000B3010000}"/>
+    <hyperlink ref="C472" r:id="rId436" xr:uid="{00000000-0004-0000-0000-0000B4010000}"/>
+    <hyperlink ref="C473" r:id="rId437" xr:uid="{00000000-0004-0000-0000-0000B5010000}"/>
+    <hyperlink ref="C474" r:id="rId438" xr:uid="{00000000-0004-0000-0000-0000B6010000}"/>
+    <hyperlink ref="C475" r:id="rId439" xr:uid="{00000000-0004-0000-0000-0000B7010000}"/>
+    <hyperlink ref="C476" r:id="rId440" xr:uid="{00000000-0004-0000-0000-0000B8010000}"/>
+    <hyperlink ref="C477" r:id="rId441" xr:uid="{00000000-0004-0000-0000-0000B9010000}"/>
+    <hyperlink ref="C478" r:id="rId442" xr:uid="{00000000-0004-0000-0000-0000BA010000}"/>
+    <hyperlink ref="C479" r:id="rId443" xr:uid="{00000000-0004-0000-0000-0000BB010000}"/>
+    <hyperlink ref="C480" r:id="rId444" location=":~:text=Given%20an%20integer%20n%2C%20calculate,*%2C%20%2F%20and%20pow().&amp;text=A%20Simple%20Solution%20is%20to%20repeatedly%20add%20n%20to%20result." xr:uid="{00000000-0004-0000-0000-0000BC010000}"/>
+    <hyperlink ref="C481" r:id="rId445" xr:uid="{00000000-0004-0000-0000-0000BD010000}"/>
+    <hyperlink ref="C140" r:id="rId446" xr:uid="{F69CB263-E96D-484E-9B8C-B1EA06EE2612}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait" r:id="rId447"/>

</xml_diff>

<commit_message>
DP wordbreak and First and last occurance
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Placements\Love-Babbar-SDE-Sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE7AA723-5814-4DC4-AF94-41DD18B2E2CF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F4EF7C3-6A09-4501-B906-3FDA1FDEF845}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1798,8 +1798,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="C52" sqref="C52"/>
+    <sheetView tabSelected="1" topLeftCell="A95" workbookViewId="0">
+      <selection activeCell="D101" sqref="D101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.1796875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2733,7 +2733,7 @@
       <c r="C72" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="D72" s="5" t="s">
+      <c r="D72" s="18" t="s">
         <v>8</v>
       </c>
     </row>
@@ -3117,7 +3117,7 @@
       <c r="C101" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="D101" s="5" t="s">
+      <c r="D101" s="18" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>